<commit_message>
Actualizacion plan de proyecto p1356
</commit_message>
<xml_diff>
--- a/Proyectos/2015/12/P1356 -CFDI+, Mario Govea _MO/Planeación/Plan_proyecto.xlsx
+++ b/Proyectos/2015/12/P1356 -CFDI+, Mario Govea _MO/Planeación/Plan_proyecto.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="989" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="989" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Presentación" sheetId="1" r:id="rId1"/>
@@ -272,9 +272,6 @@
     <t>Cronograma</t>
   </si>
   <si>
-    <t>https://contpaqi911.bitrix24.com/crm/deal/show/13404/</t>
-  </si>
-  <si>
     <t>Estimaciones</t>
   </si>
   <si>
@@ -669,6 +666,9 @@
   </si>
   <si>
     <t>mayo956@hotmail.com</t>
+  </si>
+  <si>
+    <t>https://contpaqi911.bitrix24.com/crm/deal/show/13630/</t>
   </si>
 </sst>
 </file>
@@ -1261,30 +1261,8 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="153">
+  <cellXfs count="154">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1620,6 +1598,29 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="2" applyBorder="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Hipervínculo" xfId="2" builtinId="8"/>
@@ -1993,107 +1994,107 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="22.5"/>
   <cols>
-    <col min="1" max="1" width="20" style="9"/>
-    <col min="2" max="2" width="8.85546875" style="9"/>
-    <col min="3" max="3" width="34.140625" style="9"/>
-    <col min="4" max="254" width="11.42578125" style="9"/>
-    <col min="255" max="255" width="2.7109375" style="9"/>
-    <col min="256" max="256" width="19.7109375" style="9"/>
-    <col min="257" max="257" width="8.85546875" style="9"/>
-    <col min="258" max="258" width="34.140625" style="9"/>
-    <col min="259" max="259" width="22.85546875" style="9"/>
-    <col min="260" max="510" width="11.42578125" style="9"/>
-    <col min="511" max="511" width="2.7109375" style="9"/>
-    <col min="512" max="512" width="19.7109375" style="9"/>
-    <col min="513" max="513" width="8.85546875" style="9"/>
-    <col min="514" max="514" width="34.140625" style="9"/>
-    <col min="515" max="515" width="22.85546875" style="9"/>
-    <col min="516" max="766" width="11.42578125" style="9"/>
-    <col min="767" max="767" width="2.7109375" style="9"/>
-    <col min="768" max="768" width="19.7109375" style="9"/>
-    <col min="769" max="769" width="8.85546875" style="9"/>
-    <col min="770" max="770" width="34.140625" style="9"/>
-    <col min="771" max="771" width="22.85546875" style="9"/>
-    <col min="772" max="1022" width="11.42578125" style="9"/>
+    <col min="1" max="1" width="20" style="1"/>
+    <col min="2" max="2" width="8.85546875" style="1"/>
+    <col min="3" max="3" width="34.140625" style="1"/>
+    <col min="4" max="254" width="11.42578125" style="1"/>
+    <col min="255" max="255" width="2.7109375" style="1"/>
+    <col min="256" max="256" width="19.7109375" style="1"/>
+    <col min="257" max="257" width="8.85546875" style="1"/>
+    <col min="258" max="258" width="34.140625" style="1"/>
+    <col min="259" max="259" width="22.85546875" style="1"/>
+    <col min="260" max="510" width="11.42578125" style="1"/>
+    <col min="511" max="511" width="2.7109375" style="1"/>
+    <col min="512" max="512" width="19.7109375" style="1"/>
+    <col min="513" max="513" width="8.85546875" style="1"/>
+    <col min="514" max="514" width="34.140625" style="1"/>
+    <col min="515" max="515" width="22.85546875" style="1"/>
+    <col min="516" max="766" width="11.42578125" style="1"/>
+    <col min="767" max="767" width="2.7109375" style="1"/>
+    <col min="768" max="768" width="19.7109375" style="1"/>
+    <col min="769" max="769" width="8.85546875" style="1"/>
+    <col min="770" max="770" width="34.140625" style="1"/>
+    <col min="771" max="771" width="22.85546875" style="1"/>
+    <col min="772" max="1022" width="11.42578125" style="1"/>
     <col min="1023" max="1025" width="11.42578125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="45.6" customHeight="1">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="148" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
+      <c r="B1" s="148"/>
+      <c r="C1" s="148"/>
     </row>
     <row r="2" spans="1:3" ht="26.1" customHeight="1">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="11">
+      <c r="B2" s="3">
         <v>1.1000000000000001</v>
       </c>
-      <c r="C2" s="12"/>
+      <c r="C2" s="4"/>
     </row>
     <row r="3" spans="1:3" ht="12.75" customHeight="1">
-      <c r="A3" s="13" t="s">
+      <c r="A3" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="7" t="s">
-        <v>167</v>
-      </c>
-      <c r="C3" s="7"/>
+      <c r="B3" s="146" t="s">
+        <v>166</v>
+      </c>
+      <c r="C3" s="146"/>
     </row>
     <row r="4" spans="1:3" ht="12.75" customHeight="1">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="146" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="7"/>
+      <c r="C4" s="146"/>
     </row>
     <row r="5" spans="1:3" ht="15.6" customHeight="1">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="148" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="8"/>
-      <c r="C5" s="8"/>
+      <c r="B5" s="148"/>
+      <c r="C5" s="148"/>
     </row>
     <row r="6" spans="1:3" ht="12.75" customHeight="1">
-      <c r="A6" s="13" t="s">
+      <c r="A6" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="146" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="7"/>
+      <c r="C6" s="146"/>
     </row>
     <row r="7" spans="1:3" ht="12.75" customHeight="1">
-      <c r="A7" s="13" t="s">
+      <c r="A7" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="6">
+      <c r="B7" s="145">
         <v>42339</v>
       </c>
-      <c r="C7" s="6"/>
+      <c r="C7" s="145"/>
     </row>
     <row r="8" spans="1:3" ht="12.75" customHeight="1">
-      <c r="A8" s="13" t="s">
+      <c r="A8" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="146" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="7"/>
+      <c r="C8" s="146"/>
     </row>
     <row r="9" spans="1:3">
-      <c r="A9" s="13" t="s">
+      <c r="A9" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="5">
+      <c r="B9" s="147">
         <v>42339</v>
       </c>
-      <c r="C9" s="5"/>
+      <c r="C9" s="147"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -2115,28 +2116,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AMI30"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29:B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="22.5" outlineLevelRow="1"/>
   <cols>
-    <col min="1" max="1" width="28.5703125" style="9"/>
-    <col min="2" max="2" width="57.42578125" style="9"/>
-    <col min="3" max="3" width="16.85546875" style="9"/>
-    <col min="4" max="255" width="11.42578125" style="9"/>
-    <col min="256" max="256" width="2.7109375" style="9"/>
-    <col min="257" max="257" width="28.5703125" style="9"/>
-    <col min="258" max="258" width="57.42578125" style="9"/>
-    <col min="259" max="511" width="11.42578125" style="9"/>
-    <col min="512" max="512" width="2.7109375" style="9"/>
-    <col min="513" max="513" width="28.5703125" style="9"/>
-    <col min="514" max="514" width="57.42578125" style="9"/>
-    <col min="515" max="767" width="11.42578125" style="9"/>
-    <col min="768" max="768" width="2.7109375" style="9"/>
-    <col min="769" max="769" width="28.5703125" style="9"/>
-    <col min="770" max="770" width="57.42578125" style="9"/>
-    <col min="771" max="1023" width="11.42578125" style="9"/>
+    <col min="1" max="1" width="28.5703125" style="1"/>
+    <col min="2" max="2" width="57.42578125" style="1"/>
+    <col min="3" max="3" width="16.85546875" style="1"/>
+    <col min="4" max="255" width="11.42578125" style="1"/>
+    <col min="256" max="256" width="2.7109375" style="1"/>
+    <col min="257" max="257" width="28.5703125" style="1"/>
+    <col min="258" max="258" width="57.42578125" style="1"/>
+    <col min="259" max="511" width="11.42578125" style="1"/>
+    <col min="512" max="512" width="2.7109375" style="1"/>
+    <col min="513" max="513" width="28.5703125" style="1"/>
+    <col min="514" max="514" width="57.42578125" style="1"/>
+    <col min="515" max="767" width="11.42578125" style="1"/>
+    <col min="768" max="768" width="2.7109375" style="1"/>
+    <col min="769" max="769" width="28.5703125" style="1"/>
+    <col min="770" max="770" width="57.42578125" style="1"/>
+    <col min="771" max="1023" width="11.42578125" style="1"/>
     <col min="1024" max="1025" width="11.42578125"/>
   </cols>
   <sheetData>
@@ -3166,10 +3167,10 @@
       <c r="AMI1"/>
     </row>
     <row r="2" spans="1:1023" ht="21.75" customHeight="1">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="148" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="8"/>
+      <c r="B2" s="148"/>
       <c r="C2"/>
       <c r="D2"/>
       <c r="E2"/>
@@ -4192,20 +4193,20 @@
       <c r="AMH2"/>
       <c r="AMI2"/>
     </row>
-    <row r="3" spans="1:1023" s="16" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A3" s="13" t="s">
+    <row r="3" spans="1:1023" s="8" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A3" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="14" t="str">
+      <c r="B3" s="6" t="str">
         <f>Presentación!B3</f>
         <v>P1356 -CFDI+, Mario Govea _MO</v>
       </c>
     </row>
     <row r="4" spans="1:1023" ht="12.75" customHeight="1">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="14" t="str">
+      <c r="B4" s="6" t="str">
         <f>Presentación!B4</f>
         <v>SOS Software</v>
       </c>
@@ -4213,218 +4214,223 @@
       <c r="D4"/>
     </row>
     <row r="5" spans="1:1023" ht="19.5" customHeight="1">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="148" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="8"/>
+      <c r="B5" s="148"/>
       <c r="C5"/>
       <c r="D5"/>
     </row>
     <row r="6" spans="1:1023" ht="42.75" customHeight="1">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="146" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="7"/>
+      <c r="B6" s="146"/>
       <c r="C6"/>
       <c r="D6"/>
     </row>
     <row r="7" spans="1:1023" ht="21.75" customHeight="1">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="148" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="8"/>
+      <c r="B7" s="148"/>
       <c r="C7"/>
       <c r="D7"/>
     </row>
     <row r="8" spans="1:1023" ht="146.25" customHeight="1">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="146" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="7"/>
+      <c r="B8" s="146"/>
       <c r="C8"/>
       <c r="D8"/>
     </row>
     <row r="9" spans="1:1023" ht="19.5" customHeight="1">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="148" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="8"/>
+      <c r="B9" s="148"/>
       <c r="C9"/>
       <c r="D9"/>
     </row>
     <row r="10" spans="1:1023" ht="42.6" customHeight="1" outlineLevel="1">
-      <c r="A10" s="13" t="s">
+      <c r="A10" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="14" t="s">
+      <c r="B10" s="6" t="s">
         <v>19</v>
       </c>
       <c r="C10"/>
       <c r="D10"/>
     </row>
     <row r="11" spans="1:1023" ht="29.1" customHeight="1" outlineLevel="1">
-      <c r="A11" s="13" t="s">
+      <c r="A11" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="14" t="s">
+      <c r="B11" s="6" t="s">
         <v>21</v>
       </c>
       <c r="C11"/>
       <c r="D11"/>
     </row>
     <row r="12" spans="1:1023" ht="42.75" customHeight="1" outlineLevel="1">
-      <c r="A12" s="13" t="s">
+      <c r="A12" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="14"/>
+      <c r="B12" s="6"/>
       <c r="C12"/>
       <c r="D12"/>
     </row>
     <row r="13" spans="1:1023">
-      <c r="A13" s="17"/>
-      <c r="B13" s="18"/>
+      <c r="A13" s="9"/>
+      <c r="B13" s="10"/>
       <c r="C13"/>
       <c r="D13"/>
     </row>
     <row r="14" spans="1:1023" ht="20.25" customHeight="1">
-      <c r="A14" s="8" t="s">
+      <c r="A14" s="148" t="s">
         <v>23</v>
       </c>
-      <c r="B14" s="8"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
+      <c r="B14" s="148"/>
+      <c r="C14" s="148"/>
+      <c r="D14" s="148"/>
     </row>
     <row r="15" spans="1:1023" ht="27" customHeight="1" outlineLevel="1">
-      <c r="A15" s="19" t="s">
+      <c r="A15" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="B15" s="20" t="s">
+      <c r="B15" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="C15" s="20" t="s">
+      <c r="C15" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="D15" s="20" t="s">
+      <c r="D15" s="12" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="16" spans="1:1023" outlineLevel="1">
-      <c r="A16" s="21" t="s">
+      <c r="A16" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="B16" s="14" t="s">
+      <c r="B16" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="C16" s="22">
+      <c r="C16" s="14">
         <v>42339</v>
       </c>
-      <c r="D16" s="22">
+      <c r="D16" s="14">
         <v>42339</v>
       </c>
     </row>
     <row r="17" spans="1:4" outlineLevel="1">
-      <c r="A17" s="21" t="s">
+      <c r="A17" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="B17" s="14" t="s">
+      <c r="B17" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="C17" s="22">
+      <c r="C17" s="14">
         <v>42345</v>
       </c>
-      <c r="D17" s="22">
+      <c r="D17" s="14">
         <v>42345</v>
       </c>
     </row>
     <row r="18" spans="1:4" outlineLevel="1">
-      <c r="A18" s="21" t="s">
+      <c r="A18" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="B18" s="14" t="s">
+      <c r="B18" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="C18" s="22">
+      <c r="C18" s="14">
         <v>42340</v>
       </c>
-      <c r="D18" s="15"/>
+      <c r="D18" s="7"/>
     </row>
     <row r="19" spans="1:4" outlineLevel="1">
-      <c r="A19" s="21"/>
-      <c r="B19" s="14"/>
-      <c r="C19" s="15"/>
-      <c r="D19" s="15"/>
+      <c r="A19" s="13"/>
+      <c r="B19" s="6"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="7"/>
     </row>
     <row r="20" spans="1:4" outlineLevel="1">
-      <c r="A20" s="21"/>
-      <c r="B20" s="14"/>
-      <c r="C20" s="15"/>
-      <c r="D20" s="15"/>
+      <c r="A20" s="13"/>
+      <c r="B20" s="6"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
     </row>
     <row r="21" spans="1:4" outlineLevel="1">
-      <c r="A21" s="21"/>
-      <c r="B21" s="14"/>
-      <c r="C21" s="14"/>
-      <c r="D21" s="14"/>
+      <c r="A21" s="13"/>
+      <c r="B21" s="6"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
     </row>
     <row r="22" spans="1:4">
-      <c r="A22" s="23"/>
-      <c r="B22" s="18"/>
-      <c r="C22" s="18"/>
+      <c r="A22" s="15"/>
+      <c r="B22" s="10"/>
+      <c r="C22" s="10"/>
     </row>
     <row r="23" spans="1:4" ht="15.6" customHeight="1">
-      <c r="A23" s="8" t="s">
+      <c r="A23" s="148" t="s">
         <v>34</v>
       </c>
-      <c r="B23" s="8"/>
-      <c r="C23" s="18"/>
+      <c r="B23" s="148"/>
+      <c r="C23" s="10"/>
     </row>
     <row r="24" spans="1:4" ht="59.65" customHeight="1">
-      <c r="A24" s="24" t="s">
+      <c r="A24" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="B24" s="25"/>
-      <c r="C24" s="18"/>
+      <c r="B24" s="17"/>
+      <c r="C24" s="10"/>
     </row>
     <row r="25" spans="1:4" ht="15.6" customHeight="1">
-      <c r="A25" s="8" t="s">
+      <c r="A25" s="148" t="s">
         <v>35</v>
       </c>
-      <c r="B25" s="8"/>
-      <c r="C25" s="18"/>
+      <c r="B25" s="148"/>
+      <c r="C25" s="10"/>
     </row>
     <row r="26" spans="1:4" ht="53.65" customHeight="1">
-      <c r="A26" s="4" t="s">
+      <c r="A26" s="151" t="s">
         <v>36</v>
       </c>
-      <c r="B26" s="4"/>
-      <c r="C26" s="18"/>
+      <c r="B26" s="151"/>
+      <c r="C26" s="10"/>
     </row>
     <row r="27" spans="1:4" ht="19.5" customHeight="1">
-      <c r="A27" s="8" t="s">
+      <c r="A27" s="148" t="s">
         <v>37</v>
       </c>
-      <c r="B27" s="8"/>
+      <c r="B27" s="148"/>
     </row>
     <row r="28" spans="1:4" ht="53.25" customHeight="1">
-      <c r="A28" s="3" t="s">
+      <c r="A28" s="153" t="s">
+        <v>170</v>
+      </c>
+      <c r="B28" s="149"/>
+    </row>
+    <row r="29" spans="1:4" ht="21" customHeight="1">
+      <c r="A29" s="148" t="s">
         <v>38</v>
       </c>
-      <c r="B28" s="3"/>
-    </row>
-    <row r="29" spans="1:4" ht="21" customHeight="1">
-      <c r="A29" s="8" t="s">
+      <c r="B29" s="148"/>
+    </row>
+    <row r="30" spans="1:4" ht="45.75" customHeight="1">
+      <c r="A30" s="150" t="s">
         <v>39</v>
       </c>
-      <c r="B29" s="8"/>
-    </row>
-    <row r="30" spans="1:4" ht="45.75" customHeight="1">
-      <c r="A30" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B30" s="2"/>
+      <c r="B30" s="150"/>
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A8:B8"/>
     <mergeCell ref="A27:B27"/>
     <mergeCell ref="A28:B28"/>
     <mergeCell ref="A29:B29"/>
@@ -4434,11 +4440,6 @@
     <mergeCell ref="A23:B23"/>
     <mergeCell ref="A25:B25"/>
     <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A8:B8"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A28" r:id="rId1"/>
@@ -4458,236 +4459,236 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="42" style="26"/>
-    <col min="2" max="2" width="31.140625" style="26"/>
-    <col min="3" max="3" width="34.140625" style="26"/>
-    <col min="4" max="4" width="46.5703125" style="26"/>
-    <col min="5" max="5" width="40.85546875" style="26"/>
+    <col min="1" max="1" width="42" style="18"/>
+    <col min="2" max="2" width="31.140625" style="18"/>
+    <col min="3" max="3" width="34.140625" style="18"/>
+    <col min="4" max="4" width="46.5703125" style="18"/>
+    <col min="5" max="5" width="40.85546875" style="18"/>
     <col min="6" max="1025" width="10.7109375"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15.75">
-      <c r="A1" s="27"/>
-      <c r="B1" s="27" t="s">
+      <c r="A1" s="19"/>
+      <c r="B1" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+    </row>
+    <row r="2" spans="1:5" ht="18.75">
+      <c r="A2" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-    </row>
-    <row r="2" spans="1:5" ht="18.75">
-      <c r="A2" s="28" t="s">
+      <c r="B2" s="21"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="22"/>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="23" t="s">
         <v>42</v>
       </c>
-      <c r="B2" s="29"/>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="30"/>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="31" t="s">
+      <c r="B3" s="23" t="s">
         <v>43</v>
       </c>
-      <c r="B3" s="31" t="s">
+      <c r="C3" s="23" t="s">
         <v>44</v>
       </c>
-      <c r="C3" s="31" t="s">
+      <c r="D3" s="23" t="s">
         <v>45</v>
       </c>
-      <c r="D3" s="31" t="s">
+      <c r="E3" s="24" t="s">
         <v>46</v>
       </c>
-      <c r="E3" s="32" t="s">
+    </row>
+    <row r="4" spans="1:5" ht="38.25">
+      <c r="A4" s="25" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" ht="38.25">
-      <c r="A4" s="33" t="s">
+      <c r="B4" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="25" t="s">
         <v>48</v>
       </c>
-      <c r="B4" s="33" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="33" t="s">
+      <c r="D4" s="26" t="s">
         <v>49</v>
       </c>
-      <c r="D4" s="34" t="s">
+      <c r="E4" s="27" t="s">
         <v>50</v>
       </c>
-      <c r="E4" s="35" t="s">
+    </row>
+    <row r="5" spans="1:5" ht="25.5">
+      <c r="A5" s="25" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" ht="25.5">
-      <c r="A5" s="33" t="s">
+      <c r="B5" s="25" t="s">
         <v>52</v>
       </c>
-      <c r="B5" s="33" t="s">
+      <c r="C5" s="25">
+        <v>3313482553</v>
+      </c>
+      <c r="D5" s="26" t="s">
         <v>53</v>
       </c>
-      <c r="C5" s="33">
-        <v>3313482553</v>
-      </c>
-      <c r="D5" s="34" t="s">
+      <c r="E5" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="E5" s="35" t="s">
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="25" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" s="33" t="s">
+      <c r="B6" s="25" t="s">
         <v>56</v>
       </c>
-      <c r="B6" s="33" t="s">
+      <c r="C6" s="25">
+        <v>3316367365</v>
+      </c>
+      <c r="D6" s="26" t="s">
         <v>57</v>
       </c>
-      <c r="C6" s="33">
-        <v>3316367365</v>
-      </c>
-      <c r="D6" s="34" t="s">
+      <c r="E6" s="28" t="s">
         <v>58</v>
       </c>
-      <c r="E6" s="36" t="s">
+    </row>
+    <row r="7" spans="1:5" ht="38.25">
+      <c r="A7" s="25" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" ht="38.25">
-      <c r="A7" s="33" t="s">
+      <c r="B7" s="25" t="s">
         <v>60</v>
       </c>
-      <c r="B7" s="33" t="s">
+      <c r="C7" s="25">
+        <v>3318039095</v>
+      </c>
+      <c r="D7" s="26" t="s">
         <v>61</v>
       </c>
-      <c r="C7" s="33">
-        <v>3318039095</v>
-      </c>
-      <c r="D7" s="34" t="s">
+      <c r="E7" s="28" t="s">
         <v>62</v>
       </c>
-      <c r="E7" s="36" t="s">
+    </row>
+    <row r="8" spans="1:5" ht="25.5">
+      <c r="A8" s="25" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" ht="25.5">
-      <c r="A8" s="33" t="s">
+      <c r="B8" s="25" t="s">
         <v>64</v>
       </c>
-      <c r="B8" s="33" t="s">
+      <c r="C8" s="25" t="s">
         <v>65</v>
       </c>
-      <c r="C8" s="33" t="s">
+      <c r="D8" s="26" t="s">
         <v>66</v>
       </c>
-      <c r="D8" s="34" t="s">
+      <c r="E8" s="28" t="s">
         <v>67</v>
       </c>
-      <c r="E8" s="36" t="s">
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="25" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" s="33" t="s">
+      <c r="B9" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="25">
+        <v>3312448000</v>
+      </c>
+      <c r="D9" s="26" t="s">
         <v>69</v>
       </c>
-      <c r="B9" s="33" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" s="33">
-        <v>3312448000</v>
-      </c>
-      <c r="D9" s="34" t="s">
+      <c r="E9" s="28" t="s">
         <v>70</v>
       </c>
-      <c r="E9" s="36" t="s">
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="29"/>
+      <c r="B10" s="29"/>
+      <c r="C10" s="29"/>
+      <c r="D10" s="29"/>
+      <c r="E10" s="29"/>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="29"/>
+      <c r="B11" s="29"/>
+      <c r="C11" s="29"/>
+      <c r="D11" s="29"/>
+      <c r="E11" s="29"/>
+    </row>
+    <row r="12" spans="1:5" ht="18.75">
+      <c r="A12" s="20" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10" s="37"/>
-      <c r="B10" s="37"/>
-      <c r="C10" s="37"/>
-      <c r="D10" s="37"/>
-      <c r="E10" s="37"/>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="A11" s="37"/>
-      <c r="B11" s="37"/>
-      <c r="C11" s="37"/>
-      <c r="D11" s="37"/>
-      <c r="E11" s="37"/>
-    </row>
-    <row r="12" spans="1:5" ht="18.75">
-      <c r="A12" s="28" t="s">
+      <c r="B12" s="30"/>
+      <c r="C12" s="30"/>
+      <c r="D12" s="30"/>
+      <c r="E12" s="30"/>
+    </row>
+    <row r="13" spans="1:5" ht="25.5">
+      <c r="A13" s="29" t="s">
         <v>72</v>
       </c>
-      <c r="B12" s="38"/>
-      <c r="C12" s="38"/>
-      <c r="D12" s="38"/>
-      <c r="E12" s="38"/>
-    </row>
-    <row r="13" spans="1:5" ht="25.5">
-      <c r="A13" s="37" t="s">
+      <c r="B13" s="29" t="s">
+        <v>167</v>
+      </c>
+      <c r="C13" s="29" t="s">
+        <v>168</v>
+      </c>
+      <c r="D13" s="29" t="s">
+        <v>169</v>
+      </c>
+      <c r="E13" s="31" t="s">
         <v>73</v>
       </c>
-      <c r="B13" s="37" t="s">
-        <v>168</v>
-      </c>
-      <c r="C13" s="37" t="s">
-        <v>169</v>
-      </c>
-      <c r="D13" s="37" t="s">
-        <v>170</v>
-      </c>
-      <c r="E13" s="39" t="s">
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="29"/>
+      <c r="B14" s="29"/>
+      <c r="C14" s="29"/>
+      <c r="D14" s="29"/>
+      <c r="E14" s="29"/>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="29"/>
+      <c r="B15" s="29"/>
+      <c r="C15" s="29"/>
+      <c r="D15" s="29"/>
+      <c r="E15" s="29"/>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="29"/>
+      <c r="B16" s="29"/>
+      <c r="C16" s="29"/>
+      <c r="D16" s="29"/>
+      <c r="E16" s="29"/>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="32"/>
+      <c r="B17" s="32"/>
+      <c r="C17" s="32"/>
+      <c r="D17" s="32"/>
+      <c r="E17" s="33"/>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="34" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="14" spans="1:5">
-      <c r="A14" s="37"/>
-      <c r="B14" s="37"/>
-      <c r="C14" s="37"/>
-      <c r="D14" s="37"/>
-      <c r="E14" s="37"/>
-    </row>
-    <row r="15" spans="1:5">
-      <c r="A15" s="37"/>
-      <c r="B15" s="37"/>
-      <c r="C15" s="37"/>
-      <c r="D15" s="37"/>
-      <c r="E15" s="37"/>
-    </row>
-    <row r="16" spans="1:5">
-      <c r="A16" s="37"/>
-      <c r="B16" s="37"/>
-      <c r="C16" s="37"/>
-      <c r="D16" s="37"/>
-      <c r="E16" s="37"/>
-    </row>
-    <row r="17" spans="1:5">
-      <c r="A17" s="40"/>
-      <c r="B17" s="40"/>
-      <c r="C17" s="40"/>
-      <c r="D17" s="40"/>
-      <c r="E17" s="41"/>
-    </row>
-    <row r="21" spans="1:5">
-      <c r="A21" s="42" t="s">
-        <v>75</v>
-      </c>
-      <c r="B21" s="42"/>
-      <c r="C21" s="42"/>
-      <c r="D21" s="42"/>
-      <c r="E21" s="42"/>
+      <c r="B21" s="34"/>
+      <c r="C21" s="34"/>
+      <c r="D21" s="34"/>
+      <c r="E21" s="34"/>
     </row>
     <row r="22" spans="1:5">
       <c r="A22"/>
       <c r="B22"/>
     </row>
     <row r="23" spans="1:5" ht="18.75">
-      <c r="A23" s="43"/>
-      <c r="B23" s="44" t="s">
-        <v>76</v>
+      <c r="A23" s="35"/>
+      <c r="B23" s="36" t="s">
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -4723,106 +4724,106 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15.75">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="37" t="s">
+        <v>76</v>
+      </c>
+      <c r="B1" s="38" t="s">
         <v>77</v>
       </c>
-      <c r="B1" s="46" t="s">
+      <c r="C1" s="38" t="s">
         <v>78</v>
       </c>
-      <c r="C1" s="46" t="s">
+      <c r="D1" s="38" t="s">
         <v>79</v>
       </c>
-      <c r="D1" s="46" t="s">
+      <c r="E1" s="38" t="s">
         <v>80</v>
       </c>
-      <c r="E1" s="46" t="s">
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="39">
+        <v>1</v>
+      </c>
+      <c r="B2" s="39" t="s">
+        <v>167</v>
+      </c>
+      <c r="C2" s="40" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="47">
-        <v>1</v>
-      </c>
-      <c r="B2" s="47" t="s">
-        <v>168</v>
-      </c>
-      <c r="C2" s="48" t="s">
-        <v>82</v>
-      </c>
-      <c r="D2" s="49">
+      <c r="D2" s="41">
         <v>42340</v>
       </c>
-      <c r="E2" s="50"/>
+      <c r="E2" s="42"/>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="47"/>
-      <c r="B3" s="47"/>
-      <c r="C3" s="50"/>
-      <c r="D3" s="50"/>
-      <c r="E3" s="50"/>
+      <c r="A3" s="39"/>
+      <c r="B3" s="39"/>
+      <c r="C3" s="42"/>
+      <c r="D3" s="42"/>
+      <c r="E3" s="42"/>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="47"/>
-      <c r="B4" s="47"/>
-      <c r="C4" s="47"/>
-      <c r="D4" s="47"/>
-      <c r="E4" s="47"/>
+      <c r="A4" s="39"/>
+      <c r="B4" s="39"/>
+      <c r="C4" s="39"/>
+      <c r="D4" s="39"/>
+      <c r="E4" s="39"/>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="47"/>
-      <c r="B5" s="47"/>
-      <c r="C5" s="47"/>
-      <c r="D5" s="47"/>
-      <c r="E5" s="47"/>
+      <c r="A5" s="39"/>
+      <c r="B5" s="39"/>
+      <c r="C5" s="39"/>
+      <c r="D5" s="39"/>
+      <c r="E5" s="39"/>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="47"/>
-      <c r="B6" s="47"/>
-      <c r="C6" s="47"/>
-      <c r="D6" s="47"/>
-      <c r="E6" s="47"/>
+      <c r="A6" s="39"/>
+      <c r="B6" s="39"/>
+      <c r="C6" s="39"/>
+      <c r="D6" s="39"/>
+      <c r="E6" s="39"/>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="47"/>
-      <c r="B7" s="47"/>
-      <c r="C7" s="47"/>
-      <c r="D7" s="47"/>
-      <c r="E7" s="47"/>
+      <c r="A7" s="39"/>
+      <c r="B7" s="39"/>
+      <c r="C7" s="39"/>
+      <c r="D7" s="39"/>
+      <c r="E7" s="39"/>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" s="47"/>
-      <c r="B8" s="47"/>
-      <c r="C8" s="47"/>
-      <c r="D8" s="47"/>
-      <c r="E8" s="47"/>
+      <c r="A8" s="39"/>
+      <c r="B8" s="39"/>
+      <c r="C8" s="39"/>
+      <c r="D8" s="39"/>
+      <c r="E8" s="39"/>
     </row>
     <row r="9" spans="1:5">
-      <c r="A9" s="47"/>
-      <c r="B9" s="47"/>
-      <c r="C9" s="47"/>
-      <c r="D9" s="47"/>
-      <c r="E9" s="47"/>
+      <c r="A9" s="39"/>
+      <c r="B9" s="39"/>
+      <c r="C9" s="39"/>
+      <c r="D9" s="39"/>
+      <c r="E9" s="39"/>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="47"/>
-      <c r="B10" s="47"/>
-      <c r="C10" s="47"/>
-      <c r="D10" s="47"/>
-      <c r="E10" s="47"/>
+      <c r="A10" s="39"/>
+      <c r="B10" s="39"/>
+      <c r="C10" s="39"/>
+      <c r="D10" s="39"/>
+      <c r="E10" s="39"/>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11" s="47"/>
-      <c r="B11" s="47"/>
-      <c r="C11" s="47"/>
-      <c r="D11" s="47"/>
-      <c r="E11" s="47"/>
+      <c r="A11" s="39"/>
+      <c r="B11" s="39"/>
+      <c r="C11" s="39"/>
+      <c r="D11" s="39"/>
+      <c r="E11" s="39"/>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="47"/>
-      <c r="B12" s="47"/>
-      <c r="C12" s="47"/>
-      <c r="D12" s="47"/>
-      <c r="E12" s="47"/>
+      <c r="A12" s="39"/>
+      <c r="B12" s="39"/>
+      <c r="C12" s="39"/>
+      <c r="D12" s="39"/>
+      <c r="E12" s="39"/>
     </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
@@ -4845,53 +4846,53 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="22.85546875" style="51"/>
-    <col min="2" max="2" width="19.5703125" style="51"/>
-    <col min="3" max="3" width="19.42578125" style="51"/>
-    <col min="4" max="4" width="48.28515625" style="51"/>
-    <col min="5" max="5" width="21.5703125" style="51"/>
-    <col min="6" max="250" width="11.42578125" style="51"/>
-    <col min="251" max="251" width="2.7109375" style="51"/>
-    <col min="252" max="252" width="19" style="51"/>
-    <col min="253" max="253" width="19.5703125" style="51"/>
-    <col min="254" max="254" width="14.28515625" style="51"/>
-    <col min="255" max="255" width="19.42578125" style="51"/>
-    <col min="256" max="256" width="56" style="51"/>
-    <col min="257" max="257" width="21.5703125" style="51"/>
-    <col min="258" max="258" width="23" style="51"/>
-    <col min="259" max="259" width="16.5703125" style="51"/>
-    <col min="260" max="260" width="14.28515625" style="51"/>
-    <col min="261" max="261" width="15.28515625" style="51"/>
-    <col min="262" max="506" width="11.42578125" style="51"/>
-    <col min="507" max="507" width="2.7109375" style="51"/>
-    <col min="508" max="508" width="19" style="51"/>
-    <col min="509" max="509" width="19.5703125" style="51"/>
-    <col min="510" max="510" width="14.28515625" style="51"/>
-    <col min="511" max="511" width="19.42578125" style="51"/>
-    <col min="512" max="512" width="56" style="51"/>
-    <col min="513" max="513" width="21.5703125" style="51"/>
-    <col min="514" max="514" width="23" style="51"/>
-    <col min="515" max="515" width="16.5703125" style="51"/>
-    <col min="516" max="516" width="14.28515625" style="51"/>
-    <col min="517" max="517" width="15.28515625" style="51"/>
-    <col min="518" max="762" width="11.42578125" style="51"/>
-    <col min="763" max="763" width="2.7109375" style="51"/>
-    <col min="764" max="764" width="19" style="51"/>
-    <col min="765" max="765" width="19.5703125" style="51"/>
-    <col min="766" max="766" width="14.28515625" style="51"/>
-    <col min="767" max="767" width="19.42578125" style="51"/>
-    <col min="768" max="768" width="56" style="51"/>
-    <col min="769" max="769" width="21.5703125" style="51"/>
-    <col min="770" max="770" width="23" style="51"/>
-    <col min="771" max="771" width="16.5703125" style="51"/>
-    <col min="772" max="772" width="14.28515625" style="51"/>
-    <col min="773" max="773" width="15.28515625" style="51"/>
-    <col min="774" max="1018" width="11.42578125" style="51"/>
-    <col min="1019" max="1019" width="2.7109375" style="51"/>
-    <col min="1020" max="1020" width="19" style="51"/>
-    <col min="1021" max="1021" width="19.5703125" style="51"/>
-    <col min="1022" max="1022" width="14.28515625" style="51"/>
-    <col min="1023" max="1023" width="19.42578125" style="51"/>
+    <col min="1" max="1" width="22.85546875" style="43"/>
+    <col min="2" max="2" width="19.5703125" style="43"/>
+    <col min="3" max="3" width="19.42578125" style="43"/>
+    <col min="4" max="4" width="48.28515625" style="43"/>
+    <col min="5" max="5" width="21.5703125" style="43"/>
+    <col min="6" max="250" width="11.42578125" style="43"/>
+    <col min="251" max="251" width="2.7109375" style="43"/>
+    <col min="252" max="252" width="19" style="43"/>
+    <col min="253" max="253" width="19.5703125" style="43"/>
+    <col min="254" max="254" width="14.28515625" style="43"/>
+    <col min="255" max="255" width="19.42578125" style="43"/>
+    <col min="256" max="256" width="56" style="43"/>
+    <col min="257" max="257" width="21.5703125" style="43"/>
+    <col min="258" max="258" width="23" style="43"/>
+    <col min="259" max="259" width="16.5703125" style="43"/>
+    <col min="260" max="260" width="14.28515625" style="43"/>
+    <col min="261" max="261" width="15.28515625" style="43"/>
+    <col min="262" max="506" width="11.42578125" style="43"/>
+    <col min="507" max="507" width="2.7109375" style="43"/>
+    <col min="508" max="508" width="19" style="43"/>
+    <col min="509" max="509" width="19.5703125" style="43"/>
+    <col min="510" max="510" width="14.28515625" style="43"/>
+    <col min="511" max="511" width="19.42578125" style="43"/>
+    <col min="512" max="512" width="56" style="43"/>
+    <col min="513" max="513" width="21.5703125" style="43"/>
+    <col min="514" max="514" width="23" style="43"/>
+    <col min="515" max="515" width="16.5703125" style="43"/>
+    <col min="516" max="516" width="14.28515625" style="43"/>
+    <col min="517" max="517" width="15.28515625" style="43"/>
+    <col min="518" max="762" width="11.42578125" style="43"/>
+    <col min="763" max="763" width="2.7109375" style="43"/>
+    <col min="764" max="764" width="19" style="43"/>
+    <col min="765" max="765" width="19.5703125" style="43"/>
+    <col min="766" max="766" width="14.28515625" style="43"/>
+    <col min="767" max="767" width="19.42578125" style="43"/>
+    <col min="768" max="768" width="56" style="43"/>
+    <col min="769" max="769" width="21.5703125" style="43"/>
+    <col min="770" max="770" width="23" style="43"/>
+    <col min="771" max="771" width="16.5703125" style="43"/>
+    <col min="772" max="772" width="14.28515625" style="43"/>
+    <col min="773" max="773" width="15.28515625" style="43"/>
+    <col min="774" max="1018" width="11.42578125" style="43"/>
+    <col min="1019" max="1019" width="2.7109375" style="43"/>
+    <col min="1020" max="1020" width="19" style="43"/>
+    <col min="1021" max="1021" width="19.5703125" style="43"/>
+    <col min="1022" max="1022" width="14.28515625" style="43"/>
+    <col min="1023" max="1023" width="19.42578125" style="43"/>
     <col min="1024" max="1025" width="19.42578125"/>
   </cols>
   <sheetData>
@@ -5921,13 +5922,13 @@
       <c r="AMI1"/>
     </row>
     <row r="2" spans="1:1023" ht="28.5" customHeight="1">
-      <c r="A2" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
+      <c r="A2" s="152" t="s">
+        <v>82</v>
+      </c>
+      <c r="B2" s="152"/>
+      <c r="C2" s="152"/>
+      <c r="D2" s="152"/>
+      <c r="E2" s="152"/>
       <c r="F2"/>
       <c r="G2"/>
       <c r="H2"/>
@@ -6948,20 +6949,20 @@
       <c r="AMI2"/>
     </row>
     <row r="3" spans="1:1023">
-      <c r="A3" s="52" t="s">
+      <c r="A3" s="44" t="s">
+        <v>83</v>
+      </c>
+      <c r="B3" s="44" t="s">
         <v>84</v>
       </c>
-      <c r="B3" s="52" t="s">
+      <c r="C3" s="44" t="s">
+        <v>77</v>
+      </c>
+      <c r="D3" s="44" t="s">
         <v>85</v>
       </c>
-      <c r="C3" s="52" t="s">
-        <v>78</v>
-      </c>
-      <c r="D3" s="52" t="s">
+      <c r="E3" s="44" t="s">
         <v>86</v>
-      </c>
-      <c r="E3" s="52" t="s">
-        <v>87</v>
       </c>
       <c r="F3"/>
       <c r="G3"/>
@@ -7983,11 +7984,11 @@
       <c r="AMI3"/>
     </row>
     <row r="4" spans="1:1023">
-      <c r="A4" s="53"/>
-      <c r="B4" s="53"/>
-      <c r="C4" s="54"/>
-      <c r="D4" s="54"/>
-      <c r="E4" s="55"/>
+      <c r="A4" s="45"/>
+      <c r="B4" s="45"/>
+      <c r="C4" s="46"/>
+      <c r="D4" s="46"/>
+      <c r="E4" s="47"/>
       <c r="F4"/>
       <c r="G4"/>
       <c r="H4"/>
@@ -9007,92 +9008,92 @@
       <c r="AMH4"/>
       <c r="AMI4"/>
     </row>
-    <row r="5" spans="1:1023" s="58" customFormat="1" ht="25.5">
-      <c r="A5" s="56" t="s">
+    <row r="5" spans="1:1023" s="50" customFormat="1" ht="25.5">
+      <c r="A5" s="48" t="s">
+        <v>87</v>
+      </c>
+      <c r="B5" s="49" t="s">
+        <v>52</v>
+      </c>
+      <c r="C5" s="46" t="s">
+        <v>52</v>
+      </c>
+      <c r="D5" s="46" t="s">
         <v>88</v>
       </c>
-      <c r="B5" s="57" t="s">
-        <v>53</v>
-      </c>
-      <c r="C5" s="54" t="s">
-        <v>53</v>
-      </c>
-      <c r="D5" s="54" t="s">
+      <c r="E5" s="49" t="s">
         <v>89</v>
       </c>
-      <c r="E5" s="57" t="s">
+    </row>
+    <row r="6" spans="1:1023" s="50" customFormat="1" ht="25.5">
+      <c r="A6" s="48" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="6" spans="1:1023" s="58" customFormat="1" ht="25.5">
-      <c r="A6" s="56" t="s">
+      <c r="B6" s="49"/>
+      <c r="C6" s="46" t="s">
+        <v>52</v>
+      </c>
+      <c r="D6" s="46" t="s">
         <v>91</v>
       </c>
-      <c r="B6" s="57"/>
-      <c r="C6" s="54" t="s">
-        <v>53</v>
-      </c>
-      <c r="D6" s="54" t="s">
+      <c r="E6" s="49" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1023" s="50" customFormat="1" ht="51">
+      <c r="A7" s="48" t="s">
         <v>92</v>
       </c>
-      <c r="E6" s="57" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1023" s="58" customFormat="1" ht="51">
-      <c r="A7" s="56" t="s">
+      <c r="B7" s="49" t="s">
+        <v>64</v>
+      </c>
+      <c r="C7" s="46" t="s">
         <v>93</v>
       </c>
-      <c r="B7" s="57" t="s">
-        <v>65</v>
-      </c>
-      <c r="C7" s="54" t="s">
+      <c r="D7" s="46" t="s">
         <v>94</v>
       </c>
-      <c r="D7" s="54" t="s">
+      <c r="E7" s="49" t="s">
         <v>95</v>
       </c>
-      <c r="E7" s="57" t="s">
+    </row>
+    <row r="8" spans="1:1023" s="50" customFormat="1" ht="25.5">
+      <c r="A8" s="48" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="8" spans="1:1023" s="58" customFormat="1" ht="25.5">
-      <c r="A8" s="56" t="s">
+      <c r="B8" s="49" t="s">
+        <v>60</v>
+      </c>
+      <c r="C8" s="46" t="s">
         <v>97</v>
       </c>
-      <c r="B8" s="57" t="s">
-        <v>61</v>
-      </c>
-      <c r="C8" s="54" t="s">
+      <c r="D8" s="46" t="s">
         <v>98</v>
       </c>
-      <c r="D8" s="54" t="s">
+      <c r="E8" s="49" t="s">
         <v>99</v>
       </c>
-      <c r="E8" s="57" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1023" s="58" customFormat="1">
-      <c r="A9" s="56"/>
-      <c r="B9" s="57"/>
-      <c r="C9" s="54"/>
-      <c r="D9" s="54"/>
-      <c r="E9" s="57"/>
+    </row>
+    <row r="9" spans="1:1023" s="50" customFormat="1">
+      <c r="A9" s="48"/>
+      <c r="B9" s="49"/>
+      <c r="C9" s="46"/>
+      <c r="D9" s="46"/>
+      <c r="E9" s="49"/>
     </row>
     <row r="10" spans="1:1023">
-      <c r="A10" s="56"/>
-      <c r="B10" s="57"/>
-      <c r="C10" s="54"/>
-      <c r="D10" s="57"/>
-      <c r="E10" s="57"/>
+      <c r="A10" s="48"/>
+      <c r="B10" s="49"/>
+      <c r="C10" s="46"/>
+      <c r="D10" s="49"/>
+      <c r="E10" s="49"/>
     </row>
     <row r="11" spans="1:1023">
-      <c r="A11" s="56"/>
-      <c r="B11" s="57"/>
-      <c r="C11" s="54"/>
-      <c r="D11" s="57"/>
-      <c r="E11" s="57"/>
+      <c r="A11" s="48"/>
+      <c r="B11" s="49"/>
+      <c r="C11" s="46"/>
+      <c r="D11" s="49"/>
+      <c r="E11" s="49"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -9120,16 +9121,16 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="32.42578125" style="59"/>
-    <col min="2" max="2" width="12.7109375" style="59"/>
-    <col min="3" max="3" width="22.28515625" style="59"/>
-    <col min="4" max="4" width="11.7109375" style="59"/>
-    <col min="5" max="5" width="16" style="59"/>
-    <col min="6" max="6" width="11.42578125" style="59"/>
-    <col min="7" max="7" width="26" style="59"/>
-    <col min="8" max="9" width="11.42578125" style="59"/>
-    <col min="10" max="10" width="13.7109375" style="59"/>
-    <col min="11" max="1023" width="11.42578125" style="59"/>
+    <col min="1" max="1" width="32.42578125" style="51"/>
+    <col min="2" max="2" width="12.7109375" style="51"/>
+    <col min="3" max="3" width="22.28515625" style="51"/>
+    <col min="4" max="4" width="11.7109375" style="51"/>
+    <col min="5" max="5" width="16" style="51"/>
+    <col min="6" max="6" width="11.42578125" style="51"/>
+    <col min="7" max="7" width="26" style="51"/>
+    <col min="8" max="9" width="11.42578125" style="51"/>
+    <col min="10" max="10" width="13.7109375" style="51"/>
+    <col min="11" max="1023" width="11.42578125" style="51"/>
     <col min="1024" max="1025" width="11.42578125"/>
   </cols>
   <sheetData>
@@ -9144,190 +9145,190 @@
       <c r="J1"/>
     </row>
     <row r="2" spans="1:10" ht="22.5" customHeight="1">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="148" t="s">
+        <v>100</v>
+      </c>
+      <c r="B2" s="148"/>
+      <c r="C2" s="148"/>
+      <c r="D2" s="148"/>
+      <c r="E2" s="148"/>
+      <c r="F2" s="148"/>
+      <c r="G2" s="148"/>
+      <c r="J2"/>
+    </row>
+    <row r="3" spans="1:10" ht="25.5">
+      <c r="A3" s="12" t="s">
         <v>101</v>
       </c>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="J2"/>
-    </row>
-    <row r="3" spans="1:10" ht="25.5">
-      <c r="A3" s="20" t="s">
+      <c r="B3" s="12" t="s">
         <v>102</v>
       </c>
-      <c r="B3" s="20" t="s">
+      <c r="C3" s="12" t="s">
         <v>103</v>
       </c>
-      <c r="C3" s="20" t="s">
+      <c r="D3" s="12" t="s">
         <v>104</v>
       </c>
-      <c r="D3" s="20" t="s">
+      <c r="E3" s="12" t="s">
         <v>105</v>
       </c>
-      <c r="E3" s="20" t="s">
+      <c r="F3" s="12" t="s">
         <v>106</v>
       </c>
-      <c r="F3" s="20" t="s">
+      <c r="G3" s="12" t="s">
         <v>107</v>
       </c>
-      <c r="G3" s="20" t="s">
+      <c r="J3"/>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" s="52" t="s">
         <v>108</v>
       </c>
-      <c r="J3"/>
-    </row>
-    <row r="4" spans="1:10">
-      <c r="A4" s="60" t="s">
+      <c r="B4" s="31" t="s">
         <v>109</v>
       </c>
-      <c r="B4" s="39" t="s">
+      <c r="C4" s="53" t="s">
         <v>110</v>
       </c>
-      <c r="C4" s="61" t="s">
+      <c r="D4" s="31">
+        <v>1</v>
+      </c>
+      <c r="E4" s="54"/>
+      <c r="F4" s="54" t="s">
+        <v>110</v>
+      </c>
+      <c r="G4" s="31"/>
+      <c r="J4" s="55" t="s">
         <v>111</v>
       </c>
-      <c r="D4" s="39">
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" s="52" t="s">
+        <v>112</v>
+      </c>
+      <c r="B5" s="31" t="s">
+        <v>109</v>
+      </c>
+      <c r="C5" s="53" t="s">
+        <v>110</v>
+      </c>
+      <c r="D5" s="31">
         <v>1</v>
       </c>
-      <c r="E4" s="62"/>
-      <c r="F4" s="62" t="s">
-        <v>111</v>
-      </c>
-      <c r="G4" s="39"/>
-      <c r="J4" s="63" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10">
-      <c r="A5" s="60" t="s">
+      <c r="E5" s="54"/>
+      <c r="F5" s="54" t="s">
+        <v>110</v>
+      </c>
+      <c r="G5" s="31"/>
+      <c r="J5" s="55" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="51">
+      <c r="A6" s="56" t="s">
         <v>113</v>
       </c>
-      <c r="B5" s="39" t="s">
+      <c r="B6" s="53" t="s">
+        <v>114</v>
+      </c>
+      <c r="C6" s="53" t="s">
         <v>110</v>
       </c>
-      <c r="C5" s="61" t="s">
-        <v>111</v>
-      </c>
-      <c r="D5" s="39">
-        <v>1</v>
-      </c>
-      <c r="E5" s="62"/>
-      <c r="F5" s="62" t="s">
-        <v>111</v>
-      </c>
-      <c r="G5" s="39"/>
-      <c r="J5" s="63" t="s">
+      <c r="D6" s="53">
+        <v>2</v>
+      </c>
+      <c r="E6" s="57"/>
+      <c r="F6" s="57" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" ht="51">
-      <c r="A6" s="64" t="s">
+      <c r="G6" s="53" t="s">
+        <v>115</v>
+      </c>
+      <c r="J6" s="55" t="s">
         <v>114</v>
       </c>
-      <c r="B6" s="61" t="s">
-        <v>115</v>
-      </c>
-      <c r="C6" s="61" t="s">
-        <v>111</v>
-      </c>
-      <c r="D6" s="61">
-        <v>2</v>
-      </c>
-      <c r="E6" s="65"/>
-      <c r="F6" s="65" t="s">
-        <v>111</v>
-      </c>
-      <c r="G6" s="61" t="s">
-        <v>116</v>
-      </c>
-      <c r="J6" s="63" t="s">
-        <v>115</v>
-      </c>
     </row>
     <row r="7" spans="1:10">
-      <c r="A7" s="60"/>
-      <c r="B7" s="39"/>
-      <c r="C7" s="39"/>
-      <c r="D7" s="39"/>
-      <c r="E7" s="62"/>
-      <c r="F7" s="62"/>
-      <c r="G7" s="39"/>
-      <c r="J7" s="63"/>
+      <c r="A7" s="52"/>
+      <c r="B7" s="31"/>
+      <c r="C7" s="31"/>
+      <c r="D7" s="31"/>
+      <c r="E7" s="54"/>
+      <c r="F7" s="54"/>
+      <c r="G7" s="31"/>
+      <c r="J7" s="55"/>
     </row>
     <row r="8" spans="1:10">
-      <c r="A8" s="60"/>
-      <c r="B8" s="39"/>
-      <c r="C8" s="39"/>
-      <c r="D8" s="39"/>
-      <c r="E8" s="62"/>
-      <c r="F8" s="62"/>
-      <c r="G8" s="39"/>
+      <c r="A8" s="52"/>
+      <c r="B8" s="31"/>
+      <c r="C8" s="31"/>
+      <c r="D8" s="31"/>
+      <c r="E8" s="54"/>
+      <c r="F8" s="54"/>
+      <c r="G8" s="31"/>
     </row>
     <row r="9" spans="1:10">
-      <c r="A9" s="66"/>
-      <c r="B9" s="39"/>
-      <c r="C9" s="39"/>
-      <c r="D9" s="67"/>
-      <c r="E9" s="62"/>
-      <c r="F9" s="62"/>
-      <c r="G9" s="39"/>
+      <c r="A9" s="58"/>
+      <c r="B9" s="31"/>
+      <c r="C9" s="31"/>
+      <c r="D9" s="59"/>
+      <c r="E9" s="54"/>
+      <c r="F9" s="54"/>
+      <c r="G9" s="31"/>
     </row>
     <row r="10" spans="1:10">
-      <c r="A10" s="60"/>
-      <c r="B10" s="39"/>
-      <c r="C10" s="39"/>
-      <c r="D10" s="39"/>
-      <c r="E10" s="62"/>
-      <c r="F10" s="62"/>
-      <c r="G10" s="39"/>
+      <c r="A10" s="52"/>
+      <c r="B10" s="31"/>
+      <c r="C10" s="31"/>
+      <c r="D10" s="31"/>
+      <c r="E10" s="54"/>
+      <c r="F10" s="54"/>
+      <c r="G10" s="31"/>
     </row>
     <row r="11" spans="1:10">
-      <c r="A11" s="60"/>
-      <c r="B11" s="39"/>
-      <c r="C11" s="39"/>
-      <c r="D11" s="39"/>
-      <c r="E11" s="62"/>
-      <c r="F11" s="62"/>
-      <c r="G11" s="39"/>
+      <c r="A11" s="52"/>
+      <c r="B11" s="31"/>
+      <c r="C11" s="31"/>
+      <c r="D11" s="31"/>
+      <c r="E11" s="54"/>
+      <c r="F11" s="54"/>
+      <c r="G11" s="31"/>
     </row>
     <row r="12" spans="1:10">
-      <c r="A12" s="60"/>
-      <c r="B12" s="39"/>
-      <c r="C12" s="39"/>
-      <c r="D12" s="39"/>
-      <c r="E12" s="62"/>
-      <c r="F12" s="62"/>
-      <c r="G12" s="39"/>
+      <c r="A12" s="52"/>
+      <c r="B12" s="31"/>
+      <c r="C12" s="31"/>
+      <c r="D12" s="31"/>
+      <c r="E12" s="54"/>
+      <c r="F12" s="54"/>
+      <c r="G12" s="31"/>
     </row>
     <row r="13" spans="1:10">
-      <c r="A13" s="39"/>
-      <c r="B13" s="39"/>
-      <c r="C13" s="39"/>
-      <c r="D13" s="39"/>
-      <c r="E13" s="39"/>
-      <c r="F13" s="39"/>
-      <c r="G13" s="39"/>
+      <c r="A13" s="31"/>
+      <c r="B13" s="31"/>
+      <c r="C13" s="31"/>
+      <c r="D13" s="31"/>
+      <c r="E13" s="31"/>
+      <c r="F13" s="31"/>
+      <c r="G13" s="31"/>
     </row>
     <row r="14" spans="1:10">
-      <c r="A14" s="39"/>
-      <c r="B14" s="39"/>
-      <c r="C14" s="39"/>
-      <c r="D14" s="39"/>
-      <c r="E14" s="39"/>
-      <c r="F14" s="39"/>
-      <c r="G14" s="39"/>
+      <c r="A14" s="31"/>
+      <c r="B14" s="31"/>
+      <c r="C14" s="31"/>
+      <c r="D14" s="31"/>
+      <c r="E14" s="31"/>
+      <c r="F14" s="31"/>
+      <c r="G14" s="31"/>
     </row>
     <row r="15" spans="1:10">
-      <c r="A15" s="39"/>
-      <c r="B15" s="39"/>
-      <c r="C15" s="39"/>
-      <c r="D15" s="39"/>
-      <c r="E15" s="39"/>
-      <c r="F15" s="39"/>
-      <c r="G15" s="39"/>
+      <c r="A15" s="31"/>
+      <c r="B15" s="31"/>
+      <c r="C15" s="31"/>
+      <c r="D15" s="31"/>
+      <c r="E15" s="31"/>
+      <c r="F15" s="31"/>
+      <c r="G15" s="31"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -9349,7 +9350,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:JA43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D5" workbookViewId="0">
+    <sheetView topLeftCell="D5" workbookViewId="0">
       <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
@@ -9370,1053 +9371,1053 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:261">
-      <c r="A1" s="68"/>
-      <c r="C1" s="69"/>
-      <c r="D1" s="69"/>
+      <c r="A1" s="60"/>
+      <c r="C1" s="61"/>
+      <c r="D1" s="61"/>
     </row>
     <row r="2" spans="1:261" ht="23.25">
-      <c r="A2" s="70"/>
-      <c r="B2" s="71"/>
-      <c r="C2" s="71"/>
-      <c r="D2" s="71"/>
-      <c r="E2" s="70" t="s">
+      <c r="A2" s="62"/>
+      <c r="B2" s="63"/>
+      <c r="C2" s="63"/>
+      <c r="D2" s="63"/>
+      <c r="E2" s="62" t="s">
+        <v>116</v>
+      </c>
+      <c r="F2" s="63"/>
+      <c r="G2" s="63"/>
+      <c r="H2" s="63"/>
+      <c r="I2" s="63"/>
+      <c r="J2" s="63"/>
+      <c r="K2" s="64"/>
+      <c r="IR2" s="65" t="s">
         <v>117</v>
       </c>
-      <c r="F2" s="71"/>
-      <c r="G2" s="71"/>
-      <c r="H2" s="71"/>
-      <c r="I2" s="71"/>
-      <c r="J2" s="71"/>
-      <c r="K2" s="72"/>
-      <c r="IR2" s="73" t="s">
+      <c r="IS2" s="65"/>
+      <c r="IT2" s="65"/>
+      <c r="IU2" s="65"/>
+      <c r="IV2" s="65"/>
+      <c r="IW2" s="65"/>
+      <c r="IX2" s="65"/>
+      <c r="IY2" s="65"/>
+      <c r="IZ2" s="65"/>
+      <c r="JA2" s="65"/>
+    </row>
+    <row r="3" spans="1:261">
+      <c r="A3" s="66"/>
+      <c r="B3" s="67"/>
+      <c r="C3" s="68"/>
+      <c r="D3" s="68"/>
+      <c r="E3" s="68"/>
+      <c r="F3" s="68"/>
+      <c r="G3" s="69"/>
+      <c r="H3" s="69"/>
+      <c r="I3" s="69"/>
+      <c r="J3" s="69"/>
+      <c r="K3" s="70"/>
+      <c r="AE3" s="71" t="s">
         <v>118</v>
       </c>
-      <c r="IS2" s="73"/>
-      <c r="IT2" s="73"/>
-      <c r="IU2" s="73"/>
-      <c r="IV2" s="73"/>
-      <c r="IW2" s="73"/>
-      <c r="IX2" s="73"/>
-      <c r="IY2" s="73"/>
-      <c r="IZ2" s="73"/>
-      <c r="JA2" s="73"/>
-    </row>
-    <row r="3" spans="1:261">
-      <c r="A3" s="74"/>
-      <c r="B3" s="75"/>
-      <c r="C3" s="76"/>
-      <c r="D3" s="76"/>
-      <c r="E3" s="76"/>
-      <c r="F3" s="76"/>
-      <c r="G3" s="77"/>
-      <c r="H3" s="77"/>
-      <c r="I3" s="77"/>
-      <c r="J3" s="77"/>
-      <c r="K3" s="78"/>
-      <c r="AE3" s="79" t="s">
+      <c r="AF3" s="71" t="s">
         <v>119</v>
       </c>
-      <c r="AF3" s="79" t="s">
+    </row>
+    <row r="4" spans="1:261" ht="30">
+      <c r="A4" s="72" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="4" spans="1:261" ht="30">
-      <c r="A4" s="80" t="s">
+      <c r="B4" s="73" t="s">
         <v>121</v>
       </c>
-      <c r="B4" s="81" t="s">
+      <c r="C4" s="74" t="s">
         <v>122</v>
       </c>
-      <c r="C4" s="82" t="s">
+      <c r="D4" s="74" t="s">
         <v>123</v>
       </c>
-      <c r="D4" s="82" t="s">
+      <c r="E4" s="74" t="s">
         <v>124</v>
       </c>
-      <c r="E4" s="82" t="s">
+      <c r="F4" s="74" t="s">
         <v>125</v>
       </c>
-      <c r="F4" s="82" t="s">
+      <c r="G4" s="74" t="s">
         <v>126</v>
       </c>
-      <c r="G4" s="82" t="s">
+      <c r="H4" s="74" t="s">
         <v>127</v>
       </c>
-      <c r="H4" s="82" t="s">
+      <c r="I4" s="74" t="s">
         <v>128</v>
       </c>
-      <c r="I4" s="82" t="s">
+      <c r="J4" s="75" t="s">
         <v>129</v>
       </c>
-      <c r="J4" s="83" t="s">
+      <c r="K4" s="74" t="s">
         <v>130</v>
       </c>
-      <c r="K4" s="82" t="s">
+      <c r="AE4" s="76" t="s">
+        <v>118</v>
+      </c>
+      <c r="AF4" s="76" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="5" spans="1:261" ht="76.5">
+      <c r="A5" s="77">
+        <v>1</v>
+      </c>
+      <c r="B5" s="78" t="s">
         <v>131</v>
       </c>
-      <c r="AE4" s="84" t="s">
-        <v>119</v>
-      </c>
-      <c r="AF4" s="84" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="5" spans="1:261" ht="76.5">
-      <c r="A5" s="85">
+      <c r="C5" s="77">
         <v>1</v>
       </c>
-      <c r="B5" s="86" t="s">
-        <v>132</v>
-      </c>
-      <c r="C5" s="85">
-        <v>1</v>
-      </c>
-      <c r="D5" s="87">
+      <c r="D5" s="79">
         <v>0.6</v>
       </c>
-      <c r="E5" s="85">
+      <c r="E5" s="77">
         <f>PRODUCT(A5:D5)</f>
         <v>0.6</v>
       </c>
-      <c r="F5" s="85">
+      <c r="F5" s="77">
         <v>4</v>
       </c>
-      <c r="G5" s="86" t="s">
+      <c r="G5" s="78" t="s">
+        <v>132</v>
+      </c>
+      <c r="H5" s="78" t="s">
         <v>133</v>
       </c>
-      <c r="H5" s="86" t="s">
+      <c r="I5" s="80" t="s">
+        <v>56</v>
+      </c>
+      <c r="J5" s="81" t="s">
         <v>134</v>
       </c>
-      <c r="I5" s="88" t="s">
-        <v>57</v>
-      </c>
-      <c r="J5" s="89" t="s">
+      <c r="K5" s="82" t="s">
         <v>135</v>
       </c>
-      <c r="K5" s="90" t="s">
+    </row>
+    <row r="6" spans="1:261" ht="51">
+      <c r="A6" s="77">
+        <v>2</v>
+      </c>
+      <c r="B6" s="78" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="6" spans="1:261" ht="51">
-      <c r="A6" s="85">
-        <v>2</v>
-      </c>
-      <c r="B6" s="86" t="s">
-        <v>137</v>
-      </c>
-      <c r="C6" s="85">
+      <c r="C6" s="77">
         <v>4</v>
       </c>
-      <c r="D6" s="87">
+      <c r="D6" s="79">
         <v>0.2</v>
       </c>
-      <c r="E6" s="85">
+      <c r="E6" s="77">
         <f t="shared" ref="E6:E24" si="0">PRODUCT(C6:D6)</f>
         <v>0.8</v>
       </c>
-      <c r="F6" s="85">
+      <c r="F6" s="77">
         <v>3</v>
       </c>
-      <c r="G6" s="86" t="s">
+      <c r="G6" s="78" t="s">
+        <v>137</v>
+      </c>
+      <c r="H6" s="82" t="s">
         <v>138</v>
       </c>
-      <c r="H6" s="90" t="s">
+      <c r="I6" s="80" t="s">
+        <v>56</v>
+      </c>
+      <c r="J6" s="81" t="s">
         <v>139</v>
       </c>
-      <c r="I6" s="88" t="s">
-        <v>57</v>
-      </c>
-      <c r="J6" s="89" t="s">
+      <c r="K6" s="82" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="7" spans="1:261" ht="51">
+      <c r="A7" s="77">
+        <v>3</v>
+      </c>
+      <c r="B7" s="78" t="s">
         <v>140</v>
       </c>
-      <c r="K6" s="90" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="7" spans="1:261" ht="51">
-      <c r="A7" s="85">
-        <v>3</v>
-      </c>
-      <c r="B7" s="86" t="s">
-        <v>141</v>
-      </c>
-      <c r="C7" s="85">
+      <c r="C7" s="77">
         <v>4</v>
       </c>
-      <c r="D7" s="87">
+      <c r="D7" s="79">
         <v>0.2</v>
       </c>
-      <c r="E7" s="85">
+      <c r="E7" s="77">
         <f t="shared" si="0"/>
         <v>0.8</v>
       </c>
-      <c r="F7" s="85">
+      <c r="F7" s="77">
         <v>3</v>
       </c>
-      <c r="G7" s="86" t="s">
+      <c r="G7" s="78" t="s">
+        <v>141</v>
+      </c>
+      <c r="H7" s="78" t="s">
         <v>142</v>
       </c>
-      <c r="H7" s="86" t="s">
+      <c r="I7" s="77" t="s">
+        <v>52</v>
+      </c>
+      <c r="J7" s="81" t="s">
+        <v>134</v>
+      </c>
+      <c r="K7" s="82" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="8" spans="1:261" ht="38.25">
+      <c r="A8" s="77">
+        <v>4</v>
+      </c>
+      <c r="B8" s="78" t="s">
         <v>143</v>
       </c>
-      <c r="I7" s="85" t="s">
-        <v>53</v>
-      </c>
-      <c r="J7" s="89" t="s">
-        <v>135</v>
-      </c>
-      <c r="K7" s="90" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="8" spans="1:261" ht="38.25">
-      <c r="A8" s="85">
-        <v>4</v>
-      </c>
-      <c r="B8" s="86" t="s">
-        <v>144</v>
-      </c>
-      <c r="C8" s="85">
+      <c r="C8" s="77">
         <v>5</v>
       </c>
-      <c r="D8" s="87">
+      <c r="D8" s="79">
         <v>0.01</v>
       </c>
-      <c r="E8" s="85">
+      <c r="E8" s="77">
         <f t="shared" si="0"/>
         <v>0.05</v>
       </c>
-      <c r="F8" s="85">
+      <c r="F8" s="77">
         <v>4</v>
       </c>
-      <c r="G8" s="86" t="s">
+      <c r="G8" s="78" t="s">
+        <v>144</v>
+      </c>
+      <c r="H8" s="78" t="s">
         <v>145</v>
       </c>
-      <c r="H8" s="86" t="s">
+      <c r="I8" s="77" t="s">
+        <v>10</v>
+      </c>
+      <c r="J8" s="81" t="s">
+        <v>134</v>
+      </c>
+      <c r="K8" s="82" t="s">
+        <v>110</v>
+      </c>
+      <c r="IS8" s="83"/>
+      <c r="IT8" s="84"/>
+      <c r="IU8" s="84"/>
+      <c r="IV8" s="85"/>
+      <c r="IW8" s="86"/>
+      <c r="IX8" s="86"/>
+      <c r="IY8" s="86"/>
+      <c r="IZ8" s="87"/>
+    </row>
+    <row r="9" spans="1:261" ht="58.5">
+      <c r="A9" s="77">
+        <v>5</v>
+      </c>
+      <c r="B9" s="78" t="s">
         <v>146</v>
       </c>
-      <c r="I8" s="85" t="s">
-        <v>10</v>
-      </c>
-      <c r="J8" s="89" t="s">
-        <v>135</v>
-      </c>
-      <c r="K8" s="90" t="s">
-        <v>111</v>
-      </c>
-      <c r="IS8" s="91"/>
-      <c r="IT8" s="92"/>
-      <c r="IU8" s="92"/>
-      <c r="IV8" s="93"/>
-      <c r="IW8" s="94"/>
-      <c r="IX8" s="94"/>
-      <c r="IY8" s="94"/>
-      <c r="IZ8" s="95"/>
-    </row>
-    <row r="9" spans="1:261" ht="58.5">
-      <c r="A9" s="85">
+      <c r="C9" s="77">
         <v>5</v>
       </c>
-      <c r="B9" s="86" t="s">
-        <v>147</v>
-      </c>
-      <c r="C9" s="85">
-        <v>5</v>
-      </c>
-      <c r="D9" s="87">
+      <c r="D9" s="79">
         <v>0.05</v>
       </c>
-      <c r="E9" s="85">
+      <c r="E9" s="77">
         <f t="shared" si="0"/>
         <v>0.25</v>
       </c>
-      <c r="F9" s="85">
+      <c r="F9" s="77">
         <v>4</v>
       </c>
-      <c r="G9" s="86" t="s">
+      <c r="G9" s="78" t="s">
+        <v>147</v>
+      </c>
+      <c r="H9" s="78" t="s">
         <v>148</v>
       </c>
-      <c r="H9" s="86" t="s">
+      <c r="I9" s="77" t="s">
+        <v>10</v>
+      </c>
+      <c r="J9" s="81" t="s">
         <v>149</v>
       </c>
-      <c r="I9" s="85" t="s">
-        <v>10</v>
-      </c>
-      <c r="J9" s="89" t="s">
+      <c r="K9" s="82" t="s">
+        <v>110</v>
+      </c>
+      <c r="IS9" s="88" t="s">
         <v>150</v>
       </c>
-      <c r="K9" s="90" t="s">
-        <v>111</v>
-      </c>
-      <c r="IS9" s="96" t="s">
+      <c r="IT9" s="89" t="s">
         <v>151</v>
       </c>
-      <c r="IT9" s="97" t="s">
-        <v>152</v>
-      </c>
-      <c r="IU9" s="98">
+      <c r="IU9" s="90">
         <v>0.9</v>
       </c>
-      <c r="IV9" s="99">
+      <c r="IV9" s="91">
         <f>(IV14*IU9)</f>
         <v>0.9</v>
       </c>
-      <c r="IW9" s="100">
+      <c r="IW9" s="92">
         <f>(IW14*IU9)</f>
         <v>1.8</v>
       </c>
-      <c r="IX9" s="101">
+      <c r="IX9" s="93">
         <f>(IX14*IU9)</f>
         <v>2.7</v>
       </c>
-      <c r="IY9" s="102">
+      <c r="IY9" s="94">
         <f>(IY14*IU9)</f>
         <v>3.6</v>
       </c>
-      <c r="IZ9" s="103">
+      <c r="IZ9" s="95">
         <f>(IZ14*IU9)</f>
         <v>4.5</v>
       </c>
     </row>
     <row r="10" spans="1:261" ht="38.25">
-      <c r="A10" s="104">
+      <c r="A10" s="96">
         <v>6</v>
       </c>
-      <c r="B10" s="86" t="s">
-        <v>153</v>
-      </c>
-      <c r="C10" s="85">
+      <c r="B10" s="78" t="s">
+        <v>152</v>
+      </c>
+      <c r="C10" s="77">
         <v>1</v>
       </c>
-      <c r="D10" s="87">
+      <c r="D10" s="79">
         <v>0.7</v>
       </c>
-      <c r="E10" s="85">
+      <c r="E10" s="77">
         <f t="shared" si="0"/>
         <v>0.7</v>
       </c>
-      <c r="F10" s="85">
+      <c r="F10" s="77">
         <v>3</v>
       </c>
-      <c r="G10" s="86" t="s">
+      <c r="G10" s="78" t="s">
+        <v>153</v>
+      </c>
+      <c r="H10" s="78" t="s">
         <v>154</v>
       </c>
-      <c r="H10" s="86" t="s">
+      <c r="I10" s="77" t="s">
+        <v>52</v>
+      </c>
+      <c r="J10" s="81" t="s">
         <v>155</v>
       </c>
-      <c r="I10" s="85" t="s">
-        <v>53</v>
-      </c>
-      <c r="J10" s="89" t="s">
+      <c r="K10" s="82" t="s">
+        <v>135</v>
+      </c>
+      <c r="IS10" s="88"/>
+      <c r="IT10" s="89" t="s">
         <v>156</v>
       </c>
-      <c r="K10" s="90" t="s">
-        <v>136</v>
-      </c>
-      <c r="IS10" s="96"/>
-      <c r="IT10" s="97" t="s">
-        <v>157</v>
-      </c>
-      <c r="IU10" s="98">
+      <c r="IU10" s="90">
         <v>0.7</v>
       </c>
-      <c r="IV10" s="105">
+      <c r="IV10" s="97">
         <f>(IV14*IU10)</f>
         <v>0.7</v>
       </c>
-      <c r="IW10" s="106">
+      <c r="IW10" s="98">
         <f>(IW14*IU10)</f>
         <v>1.4</v>
       </c>
-      <c r="IX10" s="107">
+      <c r="IX10" s="99">
         <f>(IX14*IU10)</f>
         <v>2.0999999999999996</v>
       </c>
-      <c r="IY10" s="108">
+      <c r="IY10" s="100">
         <f>(IY14*IU10)</f>
         <v>2.8</v>
       </c>
-      <c r="IZ10" s="109">
+      <c r="IZ10" s="101">
         <f>(IZ14*IU10)</f>
         <v>3.5</v>
       </c>
     </row>
     <row r="11" spans="1:261" ht="15">
-      <c r="A11" s="104">
+      <c r="A11" s="96">
         <v>7</v>
       </c>
-      <c r="B11" s="86"/>
-      <c r="C11" s="104"/>
-      <c r="D11" s="110"/>
-      <c r="E11" s="104">
+      <c r="B11" s="78"/>
+      <c r="C11" s="96"/>
+      <c r="D11" s="102"/>
+      <c r="E11" s="96">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F11" s="104"/>
-      <c r="G11" s="86"/>
-      <c r="H11" s="86"/>
-      <c r="I11" s="85"/>
-      <c r="J11" s="111"/>
-      <c r="K11" s="112"/>
-      <c r="IS11" s="96"/>
-      <c r="IT11" s="97" t="s">
-        <v>158</v>
-      </c>
-      <c r="IU11" s="98">
+      <c r="F11" s="96"/>
+      <c r="G11" s="78"/>
+      <c r="H11" s="78"/>
+      <c r="I11" s="77"/>
+      <c r="J11" s="103"/>
+      <c r="K11" s="104"/>
+      <c r="IS11" s="88"/>
+      <c r="IT11" s="89" t="s">
+        <v>157</v>
+      </c>
+      <c r="IU11" s="90">
         <v>0.5</v>
       </c>
-      <c r="IV11" s="105">
+      <c r="IV11" s="97">
         <f>(IV14*IU11)</f>
         <v>0.5</v>
       </c>
-      <c r="IW11" s="113">
+      <c r="IW11" s="105">
         <f>(IW14*IU11)</f>
         <v>1</v>
       </c>
-      <c r="IX11" s="106">
+      <c r="IX11" s="98">
         <f>(IX14*IU11)</f>
         <v>1.5</v>
       </c>
-      <c r="IY11" s="106">
+      <c r="IY11" s="98">
         <f>(IY14*IU11)</f>
         <v>2</v>
       </c>
-      <c r="IZ11" s="114">
+      <c r="IZ11" s="106">
         <f>(IZ14*IU11)</f>
         <v>2.5</v>
       </c>
     </row>
     <row r="12" spans="1:261" ht="15">
-      <c r="A12" s="104">
+      <c r="A12" s="96">
         <v>8</v>
       </c>
-      <c r="B12" s="86"/>
-      <c r="C12" s="104"/>
-      <c r="D12" s="110"/>
-      <c r="E12" s="104">
+      <c r="B12" s="78"/>
+      <c r="C12" s="96"/>
+      <c r="D12" s="102"/>
+      <c r="E12" s="96">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F12" s="104"/>
-      <c r="G12" s="86"/>
-      <c r="H12" s="86"/>
-      <c r="I12" s="85"/>
-      <c r="J12" s="111"/>
-      <c r="K12" s="112"/>
-      <c r="IS12" s="96"/>
-      <c r="IT12" s="97" t="s">
-        <v>159</v>
-      </c>
-      <c r="IU12" s="98">
+      <c r="F12" s="96"/>
+      <c r="G12" s="78"/>
+      <c r="H12" s="78"/>
+      <c r="I12" s="77"/>
+      <c r="J12" s="103"/>
+      <c r="K12" s="104"/>
+      <c r="IS12" s="88"/>
+      <c r="IT12" s="89" t="s">
+        <v>158</v>
+      </c>
+      <c r="IU12" s="90">
         <v>0.3</v>
       </c>
-      <c r="IV12" s="115">
+      <c r="IV12" s="107">
         <f>(IV14*IU12)</f>
         <v>0.3</v>
       </c>
-      <c r="IW12" s="116">
+      <c r="IW12" s="108">
         <f>(IW14*IU12)</f>
         <v>0.6</v>
       </c>
-      <c r="IX12" s="106">
+      <c r="IX12" s="98">
         <f>(IX14*IU12)</f>
         <v>0.89999999999999991</v>
       </c>
-      <c r="IY12" s="106">
+      <c r="IY12" s="98">
         <f>(IY14*IU12)</f>
         <v>1.2</v>
       </c>
-      <c r="IZ12" s="117">
+      <c r="IZ12" s="109">
         <f>(IZ14*IU12)</f>
         <v>1.5</v>
       </c>
     </row>
     <row r="13" spans="1:261" ht="15">
-      <c r="A13" s="104">
+      <c r="A13" s="96">
         <v>9</v>
       </c>
-      <c r="B13" s="86"/>
-      <c r="C13" s="104"/>
-      <c r="D13" s="110"/>
-      <c r="E13" s="104">
+      <c r="B13" s="78"/>
+      <c r="C13" s="96"/>
+      <c r="D13" s="102"/>
+      <c r="E13" s="96">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F13" s="104"/>
-      <c r="G13" s="118"/>
-      <c r="H13" s="86"/>
-      <c r="I13" s="85"/>
-      <c r="J13" s="111"/>
-      <c r="K13" s="112"/>
-      <c r="IS13" s="96"/>
-      <c r="IT13" s="97" t="s">
-        <v>158</v>
-      </c>
-      <c r="IU13" s="119">
+      <c r="F13" s="96"/>
+      <c r="G13" s="110"/>
+      <c r="H13" s="78"/>
+      <c r="I13" s="77"/>
+      <c r="J13" s="103"/>
+      <c r="K13" s="104"/>
+      <c r="IS13" s="88"/>
+      <c r="IT13" s="89" t="s">
+        <v>157</v>
+      </c>
+      <c r="IU13" s="111">
         <v>0.1</v>
       </c>
-      <c r="IV13" s="120">
+      <c r="IV13" s="112">
         <f>(IV14*IU13)</f>
         <v>0.1</v>
       </c>
-      <c r="IW13" s="121">
+      <c r="IW13" s="113">
         <f>(IW14*IU13)</f>
         <v>0.2</v>
       </c>
-      <c r="IX13" s="122">
+      <c r="IX13" s="114">
         <f>(IX14*IV13)</f>
         <v>0.30000000000000004</v>
       </c>
-      <c r="IY13" s="122">
+      <c r="IY13" s="114">
         <f>(IY14*IU13)</f>
         <v>0.4</v>
       </c>
-      <c r="IZ13" s="123">
+      <c r="IZ13" s="115">
         <f>(IZ14*IU13)</f>
         <v>0.5</v>
       </c>
     </row>
     <row r="14" spans="1:261" ht="15">
-      <c r="A14" s="124">
+      <c r="A14" s="116">
         <v>10</v>
       </c>
-      <c r="B14" s="125"/>
-      <c r="C14" s="124"/>
-      <c r="D14" s="126"/>
-      <c r="E14" s="124">
+      <c r="B14" s="117"/>
+      <c r="C14" s="116"/>
+      <c r="D14" s="118"/>
+      <c r="E14" s="116">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F14" s="124"/>
-      <c r="G14" s="127"/>
-      <c r="H14" s="125"/>
-      <c r="I14" s="128"/>
-      <c r="J14" s="129"/>
-      <c r="K14" s="130"/>
-      <c r="IS14" s="131"/>
-      <c r="IT14" s="132"/>
-      <c r="IU14" s="97"/>
-      <c r="IV14" s="98">
+      <c r="F14" s="116"/>
+      <c r="G14" s="119"/>
+      <c r="H14" s="117"/>
+      <c r="I14" s="120"/>
+      <c r="J14" s="121"/>
+      <c r="K14" s="122"/>
+      <c r="IS14" s="123"/>
+      <c r="IT14" s="124"/>
+      <c r="IU14" s="89"/>
+      <c r="IV14" s="90">
         <v>1</v>
       </c>
-      <c r="IW14" s="98">
+      <c r="IW14" s="90">
         <v>2</v>
       </c>
-      <c r="IX14" s="98">
+      <c r="IX14" s="90">
         <v>3</v>
       </c>
-      <c r="IY14" s="98">
+      <c r="IY14" s="90">
         <v>4</v>
       </c>
-      <c r="IZ14" s="133">
+      <c r="IZ14" s="125">
         <v>5</v>
       </c>
     </row>
     <row r="15" spans="1:261" ht="15">
-      <c r="A15" s="124">
+      <c r="A15" s="116">
         <v>11</v>
       </c>
-      <c r="B15" s="125"/>
-      <c r="C15" s="124"/>
-      <c r="D15" s="126"/>
-      <c r="E15" s="124">
+      <c r="B15" s="117"/>
+      <c r="C15" s="116"/>
+      <c r="D15" s="118"/>
+      <c r="E15" s="116">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F15" s="124"/>
-      <c r="G15" s="127"/>
-      <c r="H15" s="125"/>
-      <c r="I15" s="128"/>
-      <c r="J15" s="129"/>
-      <c r="K15" s="130"/>
-      <c r="IS15" s="131"/>
-      <c r="IT15" s="132"/>
-      <c r="IU15" s="132"/>
-      <c r="IV15" s="97" t="s">
+      <c r="F15" s="116"/>
+      <c r="G15" s="119"/>
+      <c r="H15" s="117"/>
+      <c r="I15" s="120"/>
+      <c r="J15" s="121"/>
+      <c r="K15" s="122"/>
+      <c r="IS15" s="123"/>
+      <c r="IT15" s="124"/>
+      <c r="IU15" s="124"/>
+      <c r="IV15" s="89" t="s">
+        <v>157</v>
+      </c>
+      <c r="IW15" s="89" t="s">
         <v>158</v>
       </c>
-      <c r="IW15" s="97" t="s">
+      <c r="IX15" s="89" t="s">
         <v>159</v>
       </c>
-      <c r="IX15" s="97" t="s">
-        <v>160</v>
-      </c>
-      <c r="IY15" s="97" t="s">
-        <v>157</v>
-      </c>
-      <c r="IZ15" s="134" t="s">
-        <v>152</v>
+      <c r="IY15" s="89" t="s">
+        <v>156</v>
+      </c>
+      <c r="IZ15" s="126" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="16" spans="1:261" ht="15">
-      <c r="A16" s="124">
+      <c r="A16" s="116">
         <v>12</v>
       </c>
-      <c r="B16" s="125"/>
-      <c r="C16" s="124"/>
-      <c r="D16" s="126"/>
-      <c r="E16" s="124">
+      <c r="B16" s="117"/>
+      <c r="C16" s="116"/>
+      <c r="D16" s="118"/>
+      <c r="E16" s="116">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F16" s="124"/>
-      <c r="G16" s="127"/>
-      <c r="H16" s="125"/>
-      <c r="I16" s="128"/>
-      <c r="J16" s="129"/>
-      <c r="K16" s="130"/>
-      <c r="IS16" s="131"/>
-      <c r="IT16" s="132"/>
-      <c r="IU16" s="98"/>
-      <c r="IV16" s="135" t="s">
-        <v>161</v>
-      </c>
-      <c r="IW16" s="135"/>
-      <c r="IX16" s="135"/>
-      <c r="IY16" s="135"/>
-      <c r="IZ16" s="135"/>
+      <c r="F16" s="116"/>
+      <c r="G16" s="119"/>
+      <c r="H16" s="117"/>
+      <c r="I16" s="120"/>
+      <c r="J16" s="121"/>
+      <c r="K16" s="122"/>
+      <c r="IS16" s="123"/>
+      <c r="IT16" s="124"/>
+      <c r="IU16" s="90"/>
+      <c r="IV16" s="127" t="s">
+        <v>160</v>
+      </c>
+      <c r="IW16" s="127"/>
+      <c r="IX16" s="127"/>
+      <c r="IY16" s="127"/>
+      <c r="IZ16" s="127"/>
     </row>
     <row r="17" spans="1:260" ht="15">
-      <c r="A17" s="124">
+      <c r="A17" s="116">
         <v>13</v>
       </c>
-      <c r="B17" s="125"/>
-      <c r="C17" s="124"/>
-      <c r="D17" s="126"/>
-      <c r="E17" s="124">
+      <c r="B17" s="117"/>
+      <c r="C17" s="116"/>
+      <c r="D17" s="118"/>
+      <c r="E17" s="116">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F17" s="124"/>
-      <c r="G17" s="127"/>
-      <c r="H17" s="125"/>
-      <c r="I17" s="128"/>
-      <c r="J17" s="129"/>
-      <c r="K17" s="130"/>
-      <c r="IS17" s="131"/>
-      <c r="IT17" s="132"/>
-      <c r="IU17" s="132"/>
-      <c r="IV17" s="132"/>
-      <c r="IW17" s="132"/>
-      <c r="IX17" s="132"/>
-      <c r="IY17" s="132"/>
-      <c r="IZ17" s="136"/>
+      <c r="F17" s="116"/>
+      <c r="G17" s="119"/>
+      <c r="H17" s="117"/>
+      <c r="I17" s="120"/>
+      <c r="J17" s="121"/>
+      <c r="K17" s="122"/>
+      <c r="IS17" s="123"/>
+      <c r="IT17" s="124"/>
+      <c r="IU17" s="124"/>
+      <c r="IV17" s="124"/>
+      <c r="IW17" s="124"/>
+      <c r="IX17" s="124"/>
+      <c r="IY17" s="124"/>
+      <c r="IZ17" s="128"/>
     </row>
     <row r="18" spans="1:260" ht="15">
-      <c r="A18" s="124">
+      <c r="A18" s="116">
         <v>14</v>
       </c>
-      <c r="B18" s="125"/>
-      <c r="C18" s="124"/>
-      <c r="D18" s="126"/>
-      <c r="E18" s="124">
+      <c r="B18" s="117"/>
+      <c r="C18" s="116"/>
+      <c r="D18" s="118"/>
+      <c r="E18" s="116">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F18" s="124"/>
-      <c r="G18" s="127"/>
-      <c r="H18" s="125"/>
-      <c r="I18" s="128"/>
-      <c r="J18" s="129"/>
-      <c r="K18" s="130"/>
-      <c r="IS18" s="131"/>
-      <c r="IT18" s="132"/>
-      <c r="IU18" s="137"/>
-      <c r="IV18" s="137"/>
-      <c r="IW18" s="137"/>
-      <c r="IX18" s="137"/>
-      <c r="IY18" s="137"/>
-      <c r="IZ18" s="138"/>
+      <c r="F18" s="116"/>
+      <c r="G18" s="119"/>
+      <c r="H18" s="117"/>
+      <c r="I18" s="120"/>
+      <c r="J18" s="121"/>
+      <c r="K18" s="122"/>
+      <c r="IS18" s="123"/>
+      <c r="IT18" s="124"/>
+      <c r="IU18" s="129"/>
+      <c r="IV18" s="129"/>
+      <c r="IW18" s="129"/>
+      <c r="IX18" s="129"/>
+      <c r="IY18" s="129"/>
+      <c r="IZ18" s="130"/>
     </row>
     <row r="19" spans="1:260" ht="15">
-      <c r="A19" s="124">
+      <c r="A19" s="116">
         <v>15</v>
       </c>
-      <c r="B19" s="125"/>
-      <c r="C19" s="124"/>
-      <c r="D19" s="126"/>
-      <c r="E19" s="124">
+      <c r="B19" s="117"/>
+      <c r="C19" s="116"/>
+      <c r="D19" s="118"/>
+      <c r="E19" s="116">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F19" s="124"/>
-      <c r="G19" s="127"/>
-      <c r="H19" s="125"/>
-      <c r="I19" s="128"/>
-      <c r="J19" s="129"/>
-      <c r="K19" s="130"/>
-      <c r="IS19" s="139" t="s">
-        <v>125</v>
-      </c>
-      <c r="IT19" s="139"/>
-      <c r="IU19" s="137"/>
-      <c r="IV19" s="137"/>
-      <c r="IW19" s="137"/>
-      <c r="IX19" s="137"/>
-      <c r="IY19" s="137"/>
-      <c r="IZ19" s="138"/>
+      <c r="F19" s="116"/>
+      <c r="G19" s="119"/>
+      <c r="H19" s="117"/>
+      <c r="I19" s="120"/>
+      <c r="J19" s="121"/>
+      <c r="K19" s="122"/>
+      <c r="IS19" s="131" t="s">
+        <v>124</v>
+      </c>
+      <c r="IT19" s="131"/>
+      <c r="IU19" s="129"/>
+      <c r="IV19" s="129"/>
+      <c r="IW19" s="129"/>
+      <c r="IX19" s="129"/>
+      <c r="IY19" s="129"/>
+      <c r="IZ19" s="130"/>
     </row>
     <row r="20" spans="1:260" ht="15">
-      <c r="A20" s="124">
+      <c r="A20" s="116">
         <v>16</v>
       </c>
-      <c r="B20" s="125"/>
-      <c r="C20" s="124"/>
-      <c r="D20" s="126"/>
-      <c r="E20" s="124">
+      <c r="B20" s="117"/>
+      <c r="C20" s="116"/>
+      <c r="D20" s="118"/>
+      <c r="E20" s="116">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F20" s="124"/>
-      <c r="G20" s="127"/>
-      <c r="H20" s="125"/>
-      <c r="I20" s="128"/>
-      <c r="J20" s="129"/>
-      <c r="K20" s="130"/>
-      <c r="IS20" s="140" t="s">
+      <c r="F20" s="116"/>
+      <c r="G20" s="119"/>
+      <c r="H20" s="117"/>
+      <c r="I20" s="120"/>
+      <c r="J20" s="121"/>
+      <c r="K20" s="122"/>
+      <c r="IS20" s="132" t="s">
+        <v>161</v>
+      </c>
+      <c r="IT20" s="133"/>
+      <c r="IU20" s="129"/>
+      <c r="IV20" s="134" t="s">
         <v>162</v>
       </c>
-      <c r="IT20" s="141"/>
-      <c r="IU20" s="137"/>
-      <c r="IV20" s="142" t="s">
-        <v>163</v>
-      </c>
-      <c r="IW20" s="142"/>
-      <c r="IX20" s="142"/>
-      <c r="IY20" s="142"/>
-      <c r="IZ20" s="142"/>
+      <c r="IW20" s="134"/>
+      <c r="IX20" s="134"/>
+      <c r="IY20" s="134"/>
+      <c r="IZ20" s="134"/>
     </row>
     <row r="21" spans="1:260" ht="51">
-      <c r="A21" s="124">
+      <c r="A21" s="116">
         <v>17</v>
       </c>
-      <c r="B21" s="125"/>
-      <c r="C21" s="124"/>
-      <c r="D21" s="126"/>
-      <c r="E21" s="124">
+      <c r="B21" s="117"/>
+      <c r="C21" s="116"/>
+      <c r="D21" s="118"/>
+      <c r="E21" s="116">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F21" s="124"/>
-      <c r="G21" s="127"/>
-      <c r="H21" s="125"/>
-      <c r="I21" s="128"/>
-      <c r="J21" s="129"/>
-      <c r="K21" s="130"/>
-      <c r="IS21" s="140" t="s">
+      <c r="F21" s="116"/>
+      <c r="G21" s="119"/>
+      <c r="H21" s="117"/>
+      <c r="I21" s="120"/>
+      <c r="J21" s="121"/>
+      <c r="K21" s="122"/>
+      <c r="IS21" s="132" t="s">
+        <v>163</v>
+      </c>
+      <c r="IT21" s="135"/>
+      <c r="IU21" s="129"/>
+      <c r="IV21" s="134" t="s">
         <v>164</v>
       </c>
-      <c r="IT21" s="143"/>
-      <c r="IU21" s="137"/>
-      <c r="IV21" s="142" t="s">
-        <v>165</v>
-      </c>
-      <c r="IW21" s="142"/>
-      <c r="IX21" s="142"/>
-      <c r="IY21" s="142"/>
-      <c r="IZ21" s="142"/>
+      <c r="IW21" s="134"/>
+      <c r="IX21" s="134"/>
+      <c r="IY21" s="134"/>
+      <c r="IZ21" s="134"/>
     </row>
     <row r="22" spans="1:260" ht="51">
-      <c r="A22" s="124">
+      <c r="A22" s="116">
         <v>18</v>
       </c>
-      <c r="B22" s="125"/>
-      <c r="C22" s="124"/>
-      <c r="D22" s="126"/>
-      <c r="E22" s="124">
+      <c r="B22" s="117"/>
+      <c r="C22" s="116"/>
+      <c r="D22" s="118"/>
+      <c r="E22" s="116">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F22" s="124"/>
-      <c r="G22" s="127"/>
-      <c r="H22" s="125"/>
-      <c r="I22" s="128"/>
-      <c r="J22" s="129"/>
-      <c r="K22" s="130"/>
-      <c r="IS22" s="140" t="s">
-        <v>166</v>
-      </c>
-      <c r="IT22" s="144"/>
-      <c r="IU22" s="137"/>
-      <c r="IV22" s="142" t="s">
+      <c r="F22" s="116"/>
+      <c r="G22" s="119"/>
+      <c r="H22" s="117"/>
+      <c r="I22" s="120"/>
+      <c r="J22" s="121"/>
+      <c r="K22" s="122"/>
+      <c r="IS22" s="132" t="s">
         <v>165</v>
       </c>
-      <c r="IW22" s="142"/>
-      <c r="IX22" s="142"/>
-      <c r="IY22" s="142"/>
-      <c r="IZ22" s="142"/>
+      <c r="IT22" s="136"/>
+      <c r="IU22" s="129"/>
+      <c r="IV22" s="134" t="s">
+        <v>164</v>
+      </c>
+      <c r="IW22" s="134"/>
+      <c r="IX22" s="134"/>
+      <c r="IY22" s="134"/>
+      <c r="IZ22" s="134"/>
     </row>
     <row r="23" spans="1:260" ht="15">
-      <c r="A23" s="124">
+      <c r="A23" s="116">
         <v>19</v>
       </c>
-      <c r="B23" s="125"/>
-      <c r="C23" s="124"/>
-      <c r="D23" s="126"/>
-      <c r="E23" s="124">
+      <c r="B23" s="117"/>
+      <c r="C23" s="116"/>
+      <c r="D23" s="118"/>
+      <c r="E23" s="116">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F23" s="124"/>
-      <c r="G23" s="127"/>
-      <c r="H23" s="125"/>
-      <c r="I23" s="128"/>
-      <c r="J23" s="129"/>
-      <c r="K23" s="130"/>
-      <c r="IS23" s="145"/>
-      <c r="IT23" s="146"/>
-      <c r="IU23" s="147"/>
-      <c r="IV23" s="147"/>
-      <c r="IW23" s="147"/>
-      <c r="IX23" s="147"/>
-      <c r="IY23" s="147"/>
-      <c r="IZ23" s="148"/>
+      <c r="F23" s="116"/>
+      <c r="G23" s="119"/>
+      <c r="H23" s="117"/>
+      <c r="I23" s="120"/>
+      <c r="J23" s="121"/>
+      <c r="K23" s="122"/>
+      <c r="IS23" s="137"/>
+      <c r="IT23" s="138"/>
+      <c r="IU23" s="139"/>
+      <c r="IV23" s="139"/>
+      <c r="IW23" s="139"/>
+      <c r="IX23" s="139"/>
+      <c r="IY23" s="139"/>
+      <c r="IZ23" s="140"/>
     </row>
     <row r="24" spans="1:260" ht="15">
-      <c r="A24" s="124">
+      <c r="A24" s="116">
         <v>20</v>
       </c>
-      <c r="B24" s="125"/>
-      <c r="C24" s="124"/>
-      <c r="D24" s="126"/>
-      <c r="E24" s="124">
+      <c r="B24" s="117"/>
+      <c r="C24" s="116"/>
+      <c r="D24" s="118"/>
+      <c r="E24" s="116">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F24" s="124"/>
-      <c r="G24" s="127"/>
-      <c r="H24" s="125"/>
-      <c r="I24" s="128"/>
-      <c r="J24" s="129"/>
-      <c r="K24" s="130"/>
+      <c r="F24" s="116"/>
+      <c r="G24" s="119"/>
+      <c r="H24" s="117"/>
+      <c r="I24" s="120"/>
+      <c r="J24" s="121"/>
+      <c r="K24" s="122"/>
     </row>
     <row r="25" spans="1:260">
-      <c r="A25" s="149"/>
-      <c r="B25" s="149"/>
-      <c r="C25" s="149"/>
-      <c r="D25" s="149"/>
-      <c r="E25" s="149"/>
-      <c r="F25" s="149"/>
+      <c r="A25" s="141"/>
+      <c r="B25" s="141"/>
+      <c r="C25" s="141"/>
+      <c r="D25" s="141"/>
+      <c r="E25" s="141"/>
+      <c r="F25" s="141"/>
     </row>
     <row r="26" spans="1:260">
-      <c r="A26" s="149"/>
-      <c r="B26" s="149"/>
-      <c r="C26" s="149"/>
-      <c r="D26" s="149"/>
-      <c r="E26" s="149"/>
-      <c r="F26" s="149"/>
+      <c r="A26" s="141"/>
+      <c r="B26" s="141"/>
+      <c r="C26" s="141"/>
+      <c r="D26" s="141"/>
+      <c r="E26" s="141"/>
+      <c r="F26" s="141"/>
     </row>
     <row r="27" spans="1:260">
-      <c r="A27" s="149"/>
-      <c r="B27" s="149"/>
-      <c r="C27" s="149"/>
-      <c r="D27" s="149"/>
-      <c r="E27" s="149"/>
-      <c r="F27" s="149"/>
+      <c r="A27" s="141"/>
+      <c r="B27" s="141"/>
+      <c r="C27" s="141"/>
+      <c r="D27" s="141"/>
+      <c r="E27" s="141"/>
+      <c r="F27" s="141"/>
     </row>
     <row r="28" spans="1:260">
-      <c r="A28" s="149"/>
-      <c r="B28" s="149"/>
-      <c r="C28" s="149"/>
-      <c r="D28" s="149"/>
-      <c r="E28" s="149"/>
-      <c r="F28" s="149"/>
+      <c r="A28" s="141"/>
+      <c r="B28" s="141"/>
+      <c r="C28" s="141"/>
+      <c r="D28" s="141"/>
+      <c r="E28" s="141"/>
+      <c r="F28" s="141"/>
     </row>
     <row r="29" spans="1:260">
-      <c r="A29" s="149"/>
-      <c r="B29" s="149"/>
-      <c r="C29" s="149"/>
-      <c r="D29" s="149"/>
-      <c r="E29" s="149"/>
-      <c r="F29" s="149"/>
+      <c r="A29" s="141"/>
+      <c r="B29" s="141"/>
+      <c r="C29" s="141"/>
+      <c r="D29" s="141"/>
+      <c r="E29" s="141"/>
+      <c r="F29" s="141"/>
     </row>
     <row r="30" spans="1:260">
-      <c r="A30" s="149"/>
-      <c r="B30" s="149"/>
-      <c r="C30" s="150"/>
-      <c r="D30" s="150"/>
-      <c r="E30" s="150"/>
-      <c r="F30" s="149"/>
+      <c r="A30" s="141"/>
+      <c r="B30" s="141"/>
+      <c r="C30" s="142"/>
+      <c r="D30" s="142"/>
+      <c r="E30" s="142"/>
+      <c r="F30" s="141"/>
     </row>
     <row r="38" spans="3:32">
-      <c r="C38" s="151"/>
-      <c r="D38" s="151"/>
-      <c r="G38" s="68"/>
-      <c r="H38" s="68"/>
-      <c r="I38" s="68"/>
-      <c r="J38" s="68"/>
-      <c r="K38" s="68"/>
-      <c r="L38" s="68"/>
-      <c r="M38" s="68"/>
-      <c r="N38" s="68"/>
-      <c r="O38" s="68"/>
-      <c r="P38" s="68"/>
-      <c r="Q38" s="68"/>
-      <c r="R38" s="68"/>
-      <c r="S38" s="68"/>
-      <c r="T38" s="68"/>
-      <c r="U38" s="68"/>
-      <c r="V38" s="68"/>
-      <c r="W38" s="68"/>
-      <c r="X38" s="68"/>
-      <c r="Y38" s="68"/>
-      <c r="Z38" s="68"/>
-      <c r="AA38" s="68"/>
-      <c r="AB38" s="68"/>
-      <c r="AC38" s="68"/>
-      <c r="AD38" s="68"/>
-      <c r="AE38" s="68"/>
-      <c r="AF38" s="68"/>
+      <c r="C38" s="143"/>
+      <c r="D38" s="143"/>
+      <c r="G38" s="60"/>
+      <c r="H38" s="60"/>
+      <c r="I38" s="60"/>
+      <c r="J38" s="60"/>
+      <c r="K38" s="60"/>
+      <c r="L38" s="60"/>
+      <c r="M38" s="60"/>
+      <c r="N38" s="60"/>
+      <c r="O38" s="60"/>
+      <c r="P38" s="60"/>
+      <c r="Q38" s="60"/>
+      <c r="R38" s="60"/>
+      <c r="S38" s="60"/>
+      <c r="T38" s="60"/>
+      <c r="U38" s="60"/>
+      <c r="V38" s="60"/>
+      <c r="W38" s="60"/>
+      <c r="X38" s="60"/>
+      <c r="Y38" s="60"/>
+      <c r="Z38" s="60"/>
+      <c r="AA38" s="60"/>
+      <c r="AB38" s="60"/>
+      <c r="AC38" s="60"/>
+      <c r="AD38" s="60"/>
+      <c r="AE38" s="60"/>
+      <c r="AF38" s="60"/>
     </row>
     <row r="39" spans="3:32">
-      <c r="C39" s="151"/>
-      <c r="D39" s="151"/>
-      <c r="G39" s="68"/>
-      <c r="H39" s="68"/>
-      <c r="I39" s="68"/>
-      <c r="J39" s="68"/>
-      <c r="K39" s="68"/>
-      <c r="L39" s="68"/>
-      <c r="M39" s="68"/>
-      <c r="N39" s="68"/>
-      <c r="O39" s="68"/>
-      <c r="P39" s="68"/>
-      <c r="Q39" s="68"/>
-      <c r="R39" s="68"/>
-      <c r="S39" s="68"/>
-      <c r="T39" s="68"/>
-      <c r="U39" s="68"/>
-      <c r="V39" s="68"/>
-      <c r="W39" s="68"/>
-      <c r="X39" s="68"/>
-      <c r="Y39" s="68"/>
-      <c r="Z39" s="68"/>
-      <c r="AA39" s="68"/>
-      <c r="AB39" s="68"/>
-      <c r="AC39" s="68"/>
-      <c r="AD39" s="68"/>
-      <c r="AE39" s="68"/>
-      <c r="AF39" s="68"/>
+      <c r="C39" s="143"/>
+      <c r="D39" s="143"/>
+      <c r="G39" s="60"/>
+      <c r="H39" s="60"/>
+      <c r="I39" s="60"/>
+      <c r="J39" s="60"/>
+      <c r="K39" s="60"/>
+      <c r="L39" s="60"/>
+      <c r="M39" s="60"/>
+      <c r="N39" s="60"/>
+      <c r="O39" s="60"/>
+      <c r="P39" s="60"/>
+      <c r="Q39" s="60"/>
+      <c r="R39" s="60"/>
+      <c r="S39" s="60"/>
+      <c r="T39" s="60"/>
+      <c r="U39" s="60"/>
+      <c r="V39" s="60"/>
+      <c r="W39" s="60"/>
+      <c r="X39" s="60"/>
+      <c r="Y39" s="60"/>
+      <c r="Z39" s="60"/>
+      <c r="AA39" s="60"/>
+      <c r="AB39" s="60"/>
+      <c r="AC39" s="60"/>
+      <c r="AD39" s="60"/>
+      <c r="AE39" s="60"/>
+      <c r="AF39" s="60"/>
     </row>
     <row r="40" spans="3:32">
-      <c r="C40" s="151"/>
-      <c r="D40" s="151"/>
-      <c r="G40" s="68"/>
-      <c r="H40" s="68"/>
-      <c r="I40" s="68"/>
-      <c r="J40" s="68"/>
-      <c r="K40" s="68"/>
-      <c r="L40" s="68"/>
-      <c r="M40" s="68"/>
-      <c r="N40" s="68"/>
-      <c r="O40" s="68"/>
-      <c r="P40" s="68"/>
-      <c r="Q40" s="68"/>
-      <c r="R40" s="68"/>
-      <c r="S40" s="68"/>
-      <c r="T40" s="68"/>
-      <c r="U40" s="68"/>
-      <c r="V40" s="68"/>
-      <c r="W40" s="68"/>
-      <c r="X40" s="68"/>
-      <c r="Y40" s="68"/>
-      <c r="Z40" s="68"/>
-      <c r="AA40" s="68"/>
-      <c r="AB40" s="68"/>
-      <c r="AC40" s="68"/>
-      <c r="AD40" s="68"/>
-      <c r="AE40" s="68"/>
-      <c r="AF40" s="68"/>
+      <c r="C40" s="143"/>
+      <c r="D40" s="143"/>
+      <c r="G40" s="60"/>
+      <c r="H40" s="60"/>
+      <c r="I40" s="60"/>
+      <c r="J40" s="60"/>
+      <c r="K40" s="60"/>
+      <c r="L40" s="60"/>
+      <c r="M40" s="60"/>
+      <c r="N40" s="60"/>
+      <c r="O40" s="60"/>
+      <c r="P40" s="60"/>
+      <c r="Q40" s="60"/>
+      <c r="R40" s="60"/>
+      <c r="S40" s="60"/>
+      <c r="T40" s="60"/>
+      <c r="U40" s="60"/>
+      <c r="V40" s="60"/>
+      <c r="W40" s="60"/>
+      <c r="X40" s="60"/>
+      <c r="Y40" s="60"/>
+      <c r="Z40" s="60"/>
+      <c r="AA40" s="60"/>
+      <c r="AB40" s="60"/>
+      <c r="AC40" s="60"/>
+      <c r="AD40" s="60"/>
+      <c r="AE40" s="60"/>
+      <c r="AF40" s="60"/>
     </row>
     <row r="41" spans="3:32">
-      <c r="C41" s="152"/>
-      <c r="D41" s="152"/>
-      <c r="G41" s="68"/>
-      <c r="H41" s="68"/>
-      <c r="I41" s="68"/>
-      <c r="J41" s="68"/>
-      <c r="K41" s="68"/>
-      <c r="L41" s="68"/>
-      <c r="M41" s="68"/>
-      <c r="N41" s="68"/>
-      <c r="O41" s="68"/>
-      <c r="P41" s="68"/>
-      <c r="Q41" s="68"/>
-      <c r="R41" s="68"/>
-      <c r="S41" s="68"/>
-      <c r="T41" s="68"/>
-      <c r="U41" s="68"/>
-      <c r="V41" s="68"/>
-      <c r="W41" s="68"/>
-      <c r="X41" s="68"/>
-      <c r="Y41" s="68"/>
-      <c r="Z41" s="68"/>
-      <c r="AA41" s="68"/>
-      <c r="AB41" s="68"/>
-      <c r="AC41" s="68"/>
-      <c r="AD41" s="68"/>
-      <c r="AE41" s="68"/>
-      <c r="AF41" s="68"/>
+      <c r="C41" s="144"/>
+      <c r="D41" s="144"/>
+      <c r="G41" s="60"/>
+      <c r="H41" s="60"/>
+      <c r="I41" s="60"/>
+      <c r="J41" s="60"/>
+      <c r="K41" s="60"/>
+      <c r="L41" s="60"/>
+      <c r="M41" s="60"/>
+      <c r="N41" s="60"/>
+      <c r="O41" s="60"/>
+      <c r="P41" s="60"/>
+      <c r="Q41" s="60"/>
+      <c r="R41" s="60"/>
+      <c r="S41" s="60"/>
+      <c r="T41" s="60"/>
+      <c r="U41" s="60"/>
+      <c r="V41" s="60"/>
+      <c r="W41" s="60"/>
+      <c r="X41" s="60"/>
+      <c r="Y41" s="60"/>
+      <c r="Z41" s="60"/>
+      <c r="AA41" s="60"/>
+      <c r="AB41" s="60"/>
+      <c r="AC41" s="60"/>
+      <c r="AD41" s="60"/>
+      <c r="AE41" s="60"/>
+      <c r="AF41" s="60"/>
     </row>
     <row r="42" spans="3:32">
-      <c r="C42" s="152"/>
-      <c r="D42" s="152"/>
-      <c r="G42" s="68"/>
-      <c r="H42" s="68"/>
-      <c r="I42" s="68"/>
-      <c r="J42" s="68"/>
-      <c r="K42" s="68"/>
-      <c r="L42" s="68"/>
-      <c r="M42" s="68"/>
-      <c r="N42" s="68"/>
-      <c r="O42" s="68"/>
-      <c r="P42" s="68"/>
-      <c r="Q42" s="68"/>
-      <c r="R42" s="68"/>
-      <c r="S42" s="68"/>
-      <c r="T42" s="68"/>
-      <c r="U42" s="68"/>
-      <c r="V42" s="68"/>
-      <c r="W42" s="68"/>
-      <c r="X42" s="68"/>
-      <c r="Y42" s="68"/>
-      <c r="Z42" s="68"/>
-      <c r="AA42" s="68"/>
-      <c r="AB42" s="68"/>
-      <c r="AC42" s="68"/>
-      <c r="AD42" s="68"/>
-      <c r="AE42" s="68"/>
-      <c r="AF42" s="68"/>
+      <c r="C42" s="144"/>
+      <c r="D42" s="144"/>
+      <c r="G42" s="60"/>
+      <c r="H42" s="60"/>
+      <c r="I42" s="60"/>
+      <c r="J42" s="60"/>
+      <c r="K42" s="60"/>
+      <c r="L42" s="60"/>
+      <c r="M42" s="60"/>
+      <c r="N42" s="60"/>
+      <c r="O42" s="60"/>
+      <c r="P42" s="60"/>
+      <c r="Q42" s="60"/>
+      <c r="R42" s="60"/>
+      <c r="S42" s="60"/>
+      <c r="T42" s="60"/>
+      <c r="U42" s="60"/>
+      <c r="V42" s="60"/>
+      <c r="W42" s="60"/>
+      <c r="X42" s="60"/>
+      <c r="Y42" s="60"/>
+      <c r="Z42" s="60"/>
+      <c r="AA42" s="60"/>
+      <c r="AB42" s="60"/>
+      <c r="AC42" s="60"/>
+      <c r="AD42" s="60"/>
+      <c r="AE42" s="60"/>
+      <c r="AF42" s="60"/>
     </row>
     <row r="43" spans="3:32">
-      <c r="C43" s="152"/>
-      <c r="D43" s="152"/>
-      <c r="G43" s="68"/>
-      <c r="H43" s="68"/>
-      <c r="I43" s="68"/>
-      <c r="J43" s="68"/>
-      <c r="K43" s="68"/>
-      <c r="L43" s="68"/>
-      <c r="M43" s="68"/>
-      <c r="N43" s="68"/>
-      <c r="O43" s="68"/>
-      <c r="P43" s="68"/>
-      <c r="Q43" s="68"/>
-      <c r="R43" s="68"/>
-      <c r="S43" s="68"/>
-      <c r="T43" s="68"/>
-      <c r="U43" s="68"/>
-      <c r="V43" s="68"/>
-      <c r="W43" s="68"/>
-      <c r="X43" s="68"/>
-      <c r="Y43" s="68"/>
-      <c r="Z43" s="68"/>
-      <c r="AA43" s="68"/>
-      <c r="AB43" s="68"/>
-      <c r="AC43" s="68"/>
-      <c r="AD43" s="68"/>
-      <c r="AE43" s="68"/>
-      <c r="AF43" s="68"/>
+      <c r="C43" s="144"/>
+      <c r="D43" s="144"/>
+      <c r="G43" s="60"/>
+      <c r="H43" s="60"/>
+      <c r="I43" s="60"/>
+      <c r="J43" s="60"/>
+      <c r="K43" s="60"/>
+      <c r="L43" s="60"/>
+      <c r="M43" s="60"/>
+      <c r="N43" s="60"/>
+      <c r="O43" s="60"/>
+      <c r="P43" s="60"/>
+      <c r="Q43" s="60"/>
+      <c r="R43" s="60"/>
+      <c r="S43" s="60"/>
+      <c r="T43" s="60"/>
+      <c r="U43" s="60"/>
+      <c r="V43" s="60"/>
+      <c r="W43" s="60"/>
+      <c r="X43" s="60"/>
+      <c r="Y43" s="60"/>
+      <c r="Z43" s="60"/>
+      <c r="AA43" s="60"/>
+      <c r="AB43" s="60"/>
+      <c r="AC43" s="60"/>
+      <c r="AD43" s="60"/>
+      <c r="AE43" s="60"/>
+      <c r="AF43" s="60"/>
     </row>
   </sheetData>
   <dataValidations count="3">

</xml_diff>